<commit_message>
Added Category and Products pages
</commit_message>
<xml_diff>
--- a/Inception/ProjectPlanRevised.xlsx
+++ b/Inception/ProjectPlanRevised.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CAPSTONE\Inception\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD054557-1B79-42E8-B15F-27039E4C106E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF23A195-89CF-4501-984B-F1A19634A169}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="18563" yWindow="915" windowWidth="28770" windowHeight="15570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="9" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="prevWBS" localSheetId="0">GanttChart!$A1048576</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">GanttChart!$A$1:$BN$69</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">GanttChart!$A$1:$BN$75</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">GanttChartPro!$A$1:$C$47</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">GanttChart!$4:$7</definedName>
     <definedName name="valuevx">42.314159</definedName>
@@ -451,7 +451,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="208">
   <si>
     <t>WBS</t>
   </si>
@@ -1681,9 +1681,6 @@
     <t>Add User Page UI demonstration</t>
   </si>
   <si>
-    <t>Store/Category/Item page code demonstration</t>
-  </si>
-  <si>
     <t>UI for additonal pages demonstration</t>
   </si>
   <si>
@@ -1700,6 +1697,42 @@
   </si>
   <si>
     <t>Security testing</t>
+  </si>
+  <si>
+    <t>Code Product CRUD page</t>
+  </si>
+  <si>
+    <t>2.5.2</t>
+  </si>
+  <si>
+    <t>Code Store CRUD page</t>
+  </si>
+  <si>
+    <t>2.5.3</t>
+  </si>
+  <si>
+    <t>Code Supplier CRUD</t>
+  </si>
+  <si>
+    <t>2.5.4</t>
+  </si>
+  <si>
+    <t>Code City CRUD page</t>
+  </si>
+  <si>
+    <t>2.5.5</t>
+  </si>
+  <si>
+    <t>Code Category CRUD page</t>
+  </si>
+  <si>
+    <t>2.5.6</t>
+  </si>
+  <si>
+    <t>Code Shipping Company CRUD page</t>
+  </si>
+  <si>
+    <t>Store/Product page code demonstration</t>
   </si>
 </sst>
 </file>
@@ -3872,11 +3905,11 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CI69"/>
+  <dimension ref="A1:CI75"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AX7" sqref="AX7"/>
+      <pane ySplit="7" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4906,7 +4939,7 @@
       <c r="G8" s="73"/>
       <c r="H8" s="74"/>
       <c r="I8" s="75" t="str">
-        <f t="shared" ref="I8:I69" si="31">IF(OR(F8=0,E8=0)," - ",NETWORKDAYS(E8,F8))</f>
+        <f t="shared" ref="I8:I75" si="31">IF(OR(F8=0,E8=0)," - ",NETWORKDAYS(E8,F8))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J8" s="78"/>
@@ -5070,7 +5103,7 @@
         <v>43864</v>
       </c>
       <c r="F10" s="83">
-        <f t="shared" ref="F10:F40" si="33">IF(ISBLANK(E10)," - ",IF(G10=0,E10,E10+G10-1))</f>
+        <f t="shared" ref="F10:F46" si="33">IF(ISBLANK(E10)," - ",IF(G10=0,E10,E10+G10-1))</f>
         <v>43865</v>
       </c>
       <c r="G10" s="58">
@@ -6098,11 +6131,11 @@
       </c>
       <c r="D22" s="107"/>
       <c r="E22" s="82">
-        <v>43885</v>
+        <v>43892</v>
       </c>
       <c r="F22" s="83">
         <f t="shared" si="33"/>
-        <v>43889</v>
+        <v>43896</v>
       </c>
       <c r="G22" s="58">
         <v>5</v>
@@ -6177,18 +6210,17 @@
         <v>162</v>
       </c>
       <c r="B23" s="106" t="s">
-        <v>161</v>
+        <v>196</v>
       </c>
       <c r="C23" s="57" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D23" s="107"/>
       <c r="E23" s="82">
-        <v>43899</v>
+        <v>43892</v>
       </c>
       <c r="F23" s="83">
-        <f t="shared" si="33"/>
-        <v>43903</v>
+        <v>43896</v>
       </c>
       <c r="G23" s="58">
         <v>5</v>
@@ -6197,7 +6229,6 @@
         <v>0</v>
       </c>
       <c r="I23" s="60">
-        <f t="shared" si="31"/>
         <v>5</v>
       </c>
       <c r="J23" s="79"/>
@@ -6258,23 +6289,22 @@
       <c r="BM23" s="87"/>
       <c r="BN23" s="87"/>
     </row>
-    <row r="24" spans="1:66" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A24" s="56">
-        <v>2.6</v>
+    <row r="24" spans="1:66" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A24" s="56" t="s">
+        <v>197</v>
       </c>
       <c r="B24" s="106" t="s">
-        <v>157</v>
+        <v>198</v>
       </c>
       <c r="C24" s="57" t="s">
         <v>138</v>
       </c>
       <c r="D24" s="107"/>
       <c r="E24" s="82">
-        <v>43899</v>
+        <v>43892</v>
       </c>
       <c r="F24" s="83">
-        <f t="shared" si="33"/>
-        <v>43903</v>
+        <v>43896</v>
       </c>
       <c r="G24" s="58">
         <v>5</v>
@@ -6283,7 +6313,6 @@
         <v>0</v>
       </c>
       <c r="I24" s="60">
-        <f t="shared" si="31"/>
         <v>5</v>
       </c>
       <c r="J24" s="79"/>
@@ -6345,11 +6374,11 @@
       <c r="BN24" s="87"/>
     </row>
     <row r="25" spans="1:66" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A25" s="56">
-        <v>2.7</v>
+      <c r="A25" s="56" t="s">
+        <v>199</v>
       </c>
       <c r="B25" s="106" t="s">
-        <v>147</v>
+        <v>200</v>
       </c>
       <c r="C25" s="57" t="s">
         <v>138</v>
@@ -6359,7 +6388,6 @@
         <v>43899</v>
       </c>
       <c r="F25" s="83">
-        <f t="shared" si="33"/>
         <v>43903</v>
       </c>
       <c r="G25" s="58">
@@ -6369,7 +6397,6 @@
         <v>0</v>
       </c>
       <c r="I25" s="60">
-        <f t="shared" si="31"/>
         <v>5</v>
       </c>
       <c r="J25" s="79"/>
@@ -6431,34 +6458,32 @@
       <c r="BN25" s="87"/>
     </row>
     <row r="26" spans="1:66" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A26" s="56">
-        <v>2.8</v>
+      <c r="A26" s="56" t="s">
+        <v>201</v>
       </c>
       <c r="B26" s="106" t="s">
-        <v>158</v>
+        <v>202</v>
       </c>
       <c r="C26" s="57" t="s">
         <v>138</v>
       </c>
-      <c r="D26" s="141"/>
-      <c r="E26" s="142">
-        <v>43906</v>
-      </c>
-      <c r="F26" s="143">
-        <f t="shared" si="33"/>
-        <v>43910</v>
-      </c>
-      <c r="G26" s="144">
+      <c r="D26" s="107"/>
+      <c r="E26" s="82">
+        <v>43899</v>
+      </c>
+      <c r="F26" s="83">
+        <v>43903</v>
+      </c>
+      <c r="G26" s="58">
         <v>5</v>
       </c>
-      <c r="H26" s="145">
+      <c r="H26" s="59">
         <v>0</v>
       </c>
-      <c r="I26" s="146">
-        <f t="shared" si="31"/>
+      <c r="I26" s="60">
         <v>5</v>
       </c>
-      <c r="J26" s="147"/>
+      <c r="J26" s="79"/>
       <c r="K26" s="87"/>
       <c r="L26" s="87"/>
       <c r="M26" s="87"/>
@@ -6516,102 +6541,106 @@
       <c r="BM26" s="87"/>
       <c r="BN26" s="87"/>
     </row>
-    <row r="27" spans="1:66" s="51" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A27" s="49" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>3</v>
-      </c>
-      <c r="B27" s="50" t="s">
-        <v>148</v>
-      </c>
-      <c r="D27" s="52"/>
-      <c r="E27" s="84"/>
-      <c r="F27" s="84" t="str">
-        <f t="shared" si="33"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G27" s="53"/>
-      <c r="H27" s="54"/>
-      <c r="I27" s="55" t="str">
-        <f t="shared" si="31"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J27" s="80"/>
-      <c r="K27" s="89"/>
-      <c r="L27" s="89"/>
-      <c r="M27" s="89"/>
-      <c r="N27" s="89"/>
-      <c r="O27" s="89"/>
-      <c r="P27" s="89"/>
-      <c r="Q27" s="89"/>
-      <c r="R27" s="89"/>
-      <c r="S27" s="89"/>
-      <c r="T27" s="89"/>
-      <c r="U27" s="89"/>
-      <c r="V27" s="89"/>
-      <c r="W27" s="89"/>
-      <c r="X27" s="89"/>
-      <c r="Y27" s="89"/>
-      <c r="Z27" s="89"/>
-      <c r="AA27" s="89"/>
-      <c r="AB27" s="89"/>
-      <c r="AC27" s="89"/>
-      <c r="AD27" s="89"/>
-      <c r="AE27" s="89"/>
-      <c r="AF27" s="89"/>
-      <c r="AG27" s="89"/>
-      <c r="AH27" s="89"/>
-      <c r="AI27" s="89"/>
-      <c r="AJ27" s="89"/>
-      <c r="AK27" s="89"/>
-      <c r="AL27" s="89"/>
-      <c r="AM27" s="89"/>
-      <c r="AN27" s="89"/>
-      <c r="AO27" s="89"/>
-      <c r="AP27" s="89"/>
-      <c r="AQ27" s="89"/>
-      <c r="AR27" s="89"/>
-      <c r="AS27" s="89"/>
-      <c r="AT27" s="89"/>
-      <c r="AU27" s="89"/>
-      <c r="AV27" s="89"/>
-      <c r="AW27" s="89"/>
-      <c r="AX27" s="89"/>
-      <c r="AY27" s="89"/>
-      <c r="AZ27" s="89"/>
-      <c r="BA27" s="89"/>
-      <c r="BB27" s="89"/>
-      <c r="BC27" s="89"/>
-      <c r="BD27" s="89"/>
-      <c r="BE27" s="89"/>
-      <c r="BF27" s="89"/>
-      <c r="BG27" s="89"/>
-      <c r="BH27" s="89"/>
-      <c r="BI27" s="89"/>
-      <c r="BJ27" s="89"/>
-      <c r="BK27" s="89"/>
-      <c r="BL27" s="89"/>
-      <c r="BM27" s="89"/>
-      <c r="BN27" s="89"/>
-    </row>
-    <row r="28" spans="1:66" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A28" s="56" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>3.1</v>
+    <row r="27" spans="1:66" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A27" s="56" t="s">
+        <v>203</v>
+      </c>
+      <c r="B27" s="106" t="s">
+        <v>204</v>
+      </c>
+      <c r="C27" s="57" t="s">
+        <v>138</v>
+      </c>
+      <c r="D27" s="107"/>
+      <c r="E27" s="82">
+        <v>43899</v>
+      </c>
+      <c r="F27" s="83">
+        <v>43903</v>
+      </c>
+      <c r="G27" s="58">
+        <v>5</v>
+      </c>
+      <c r="H27" s="59">
+        <v>0</v>
+      </c>
+      <c r="I27" s="60">
+        <v>5</v>
+      </c>
+      <c r="J27" s="79"/>
+      <c r="K27" s="87"/>
+      <c r="L27" s="87"/>
+      <c r="M27" s="87"/>
+      <c r="N27" s="87"/>
+      <c r="O27" s="87"/>
+      <c r="P27" s="87"/>
+      <c r="Q27" s="87"/>
+      <c r="R27" s="87"/>
+      <c r="S27" s="87"/>
+      <c r="T27" s="87"/>
+      <c r="U27" s="87"/>
+      <c r="V27" s="87"/>
+      <c r="W27" s="87"/>
+      <c r="X27" s="87"/>
+      <c r="Y27" s="87"/>
+      <c r="Z27" s="87"/>
+      <c r="AA27" s="87"/>
+      <c r="AB27" s="87"/>
+      <c r="AC27" s="87"/>
+      <c r="AD27" s="87"/>
+      <c r="AE27" s="87"/>
+      <c r="AF27" s="87"/>
+      <c r="AG27" s="87"/>
+      <c r="AH27" s="87"/>
+      <c r="AI27" s="87"/>
+      <c r="AJ27" s="87"/>
+      <c r="AK27" s="87"/>
+      <c r="AL27" s="87"/>
+      <c r="AM27" s="87"/>
+      <c r="AN27" s="87"/>
+      <c r="AO27" s="87"/>
+      <c r="AP27" s="87"/>
+      <c r="AQ27" s="87"/>
+      <c r="AR27" s="87"/>
+      <c r="AS27" s="87"/>
+      <c r="AT27" s="87"/>
+      <c r="AU27" s="87"/>
+      <c r="AV27" s="87"/>
+      <c r="AW27" s="87"/>
+      <c r="AX27" s="87"/>
+      <c r="AY27" s="87"/>
+      <c r="AZ27" s="87"/>
+      <c r="BA27" s="87"/>
+      <c r="BB27" s="87"/>
+      <c r="BC27" s="87"/>
+      <c r="BD27" s="87"/>
+      <c r="BE27" s="87"/>
+      <c r="BF27" s="87"/>
+      <c r="BG27" s="87"/>
+      <c r="BH27" s="87"/>
+      <c r="BI27" s="87"/>
+      <c r="BJ27" s="87"/>
+      <c r="BK27" s="87"/>
+      <c r="BL27" s="87"/>
+      <c r="BM27" s="87"/>
+      <c r="BN27" s="87"/>
+    </row>
+    <row r="28" spans="1:66" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A28" s="56" t="s">
+        <v>205</v>
       </c>
       <c r="B28" s="106" t="s">
-        <v>149</v>
+        <v>206</v>
       </c>
       <c r="C28" s="57" t="s">
         <v>138</v>
       </c>
       <c r="D28" s="107"/>
       <c r="E28" s="82">
-        <v>43871</v>
+        <v>43899</v>
       </c>
       <c r="F28" s="83">
-        <f t="shared" si="33"/>
-        <v>43875</v>
+        <v>43903</v>
       </c>
       <c r="G28" s="58">
         <v>5</v>
@@ -6620,7 +6649,6 @@
         <v>0</v>
       </c>
       <c r="I28" s="60">
-        <f t="shared" si="31"/>
         <v>5</v>
       </c>
       <c r="J28" s="79"/>
@@ -6681,24 +6709,23 @@
       <c r="BM28" s="87"/>
       <c r="BN28" s="87"/>
     </row>
-    <row r="29" spans="1:66" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A29" s="56" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>3.2</v>
+    <row r="29" spans="1:66" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A29" s="56" t="s">
+        <v>162</v>
       </c>
       <c r="B29" s="106" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="C29" s="57" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D29" s="107"/>
       <c r="E29" s="82">
-        <v>43878</v>
+        <v>43906</v>
       </c>
       <c r="F29" s="83">
         <f t="shared" si="33"/>
-        <v>43882</v>
+        <v>43910</v>
       </c>
       <c r="G29" s="58">
         <v>5</v>
@@ -6768,32 +6795,33 @@
       <c r="BM29" s="87"/>
       <c r="BN29" s="87"/>
     </row>
-    <row r="30" spans="1:66" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:66" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" s="56">
-        <v>3.3</v>
+        <v>2.6</v>
       </c>
       <c r="B30" s="106" t="s">
-        <v>184</v>
+        <v>157</v>
       </c>
       <c r="C30" s="57" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D30" s="107"/>
       <c r="E30" s="82">
-        <v>43874</v>
+        <v>43913</v>
       </c>
       <c r="F30" s="83">
-        <v>43875</v>
+        <f t="shared" si="33"/>
+        <v>43917</v>
       </c>
       <c r="G30" s="58">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H30" s="59">
         <v>0</v>
       </c>
       <c r="I30" s="60">
         <f t="shared" si="31"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J30" s="79"/>
       <c r="K30" s="87"/>
@@ -6853,31 +6881,32 @@
       <c r="BM30" s="87"/>
       <c r="BN30" s="87"/>
     </row>
-    <row r="31" spans="1:66" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:66" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" s="56">
-        <v>3.4</v>
+        <v>2.7</v>
       </c>
       <c r="B31" s="106" t="s">
-        <v>185</v>
+        <v>147</v>
       </c>
       <c r="C31" s="57" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D31" s="107"/>
       <c r="E31" s="82">
-        <v>43881</v>
+        <v>43906</v>
       </c>
       <c r="F31" s="83">
-        <v>43882</v>
+        <v>43910</v>
       </c>
       <c r="G31" s="58">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H31" s="59">
         <v>0</v>
       </c>
       <c r="I31" s="60">
-        <v>2</v>
+        <f t="shared" si="31"/>
+        <v>5</v>
       </c>
       <c r="J31" s="79"/>
       <c r="K31" s="87"/>
@@ -6937,33 +6966,35 @@
       <c r="BM31" s="87"/>
       <c r="BN31" s="87"/>
     </row>
-    <row r="32" spans="1:66" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:66" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" s="56">
-        <v>3.5</v>
+        <v>2.8</v>
       </c>
       <c r="B32" s="106" t="s">
-        <v>186</v>
+        <v>158</v>
       </c>
       <c r="C32" s="57" t="s">
         <v>138</v>
       </c>
-      <c r="D32" s="107"/>
-      <c r="E32" s="82">
-        <v>43889</v>
-      </c>
-      <c r="F32" s="83">
-        <v>43889</v>
-      </c>
-      <c r="G32" s="58">
-        <v>1</v>
-      </c>
-      <c r="H32" s="59">
+      <c r="D32" s="141"/>
+      <c r="E32" s="142">
+        <v>43913</v>
+      </c>
+      <c r="F32" s="143">
+        <f t="shared" si="33"/>
+        <v>43917</v>
+      </c>
+      <c r="G32" s="144">
+        <v>5</v>
+      </c>
+      <c r="H32" s="145">
         <v>0</v>
       </c>
-      <c r="I32" s="60">
-        <v>1</v>
-      </c>
-      <c r="J32" s="79"/>
+      <c r="I32" s="146">
+        <f t="shared" si="31"/>
+        <v>5</v>
+      </c>
+      <c r="J32" s="147"/>
       <c r="K32" s="87"/>
       <c r="L32" s="87"/>
       <c r="M32" s="87"/>
@@ -7021,120 +7052,112 @@
       <c r="BM32" s="87"/>
       <c r="BN32" s="87"/>
     </row>
-    <row r="33" spans="1:66" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A33" s="56" t="str">
+    <row r="33" spans="1:66" s="51" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A33" s="49" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>3</v>
+      </c>
+      <c r="B33" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="D33" s="52"/>
+      <c r="E33" s="84"/>
+      <c r="F33" s="84" t="str">
+        <f t="shared" si="33"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G33" s="53"/>
+      <c r="H33" s="54"/>
+      <c r="I33" s="55" t="str">
+        <f t="shared" si="31"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J33" s="80"/>
+      <c r="K33" s="89"/>
+      <c r="L33" s="89"/>
+      <c r="M33" s="89"/>
+      <c r="N33" s="89"/>
+      <c r="O33" s="89"/>
+      <c r="P33" s="89"/>
+      <c r="Q33" s="89"/>
+      <c r="R33" s="89"/>
+      <c r="S33" s="89"/>
+      <c r="T33" s="89"/>
+      <c r="U33" s="89"/>
+      <c r="V33" s="89"/>
+      <c r="W33" s="89"/>
+      <c r="X33" s="89"/>
+      <c r="Y33" s="89"/>
+      <c r="Z33" s="89"/>
+      <c r="AA33" s="89"/>
+      <c r="AB33" s="89"/>
+      <c r="AC33" s="89"/>
+      <c r="AD33" s="89"/>
+      <c r="AE33" s="89"/>
+      <c r="AF33" s="89"/>
+      <c r="AG33" s="89"/>
+      <c r="AH33" s="89"/>
+      <c r="AI33" s="89"/>
+      <c r="AJ33" s="89"/>
+      <c r="AK33" s="89"/>
+      <c r="AL33" s="89"/>
+      <c r="AM33" s="89"/>
+      <c r="AN33" s="89"/>
+      <c r="AO33" s="89"/>
+      <c r="AP33" s="89"/>
+      <c r="AQ33" s="89"/>
+      <c r="AR33" s="89"/>
+      <c r="AS33" s="89"/>
+      <c r="AT33" s="89"/>
+      <c r="AU33" s="89"/>
+      <c r="AV33" s="89"/>
+      <c r="AW33" s="89"/>
+      <c r="AX33" s="89"/>
+      <c r="AY33" s="89"/>
+      <c r="AZ33" s="89"/>
+      <c r="BA33" s="89"/>
+      <c r="BB33" s="89"/>
+      <c r="BC33" s="89"/>
+      <c r="BD33" s="89"/>
+      <c r="BE33" s="89"/>
+      <c r="BF33" s="89"/>
+      <c r="BG33" s="89"/>
+      <c r="BH33" s="89"/>
+      <c r="BI33" s="89"/>
+      <c r="BJ33" s="89"/>
+      <c r="BK33" s="89"/>
+      <c r="BL33" s="89"/>
+      <c r="BM33" s="89"/>
+      <c r="BN33" s="89"/>
+    </row>
+    <row r="34" spans="1:66" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A34" s="56" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>3.6</v>
-      </c>
-      <c r="B33" s="106" t="s">
-        <v>152</v>
-      </c>
-      <c r="C33" s="57" t="s">
-        <v>153</v>
-      </c>
-      <c r="D33" s="107"/>
-      <c r="E33" s="82">
-        <v>43885</v>
-      </c>
-      <c r="F33" s="83">
+        <v>3.1</v>
+      </c>
+      <c r="B34" s="106" t="s">
+        <v>149</v>
+      </c>
+      <c r="C34" s="57" t="s">
+        <v>138</v>
+      </c>
+      <c r="D34" s="107"/>
+      <c r="E34" s="82">
+        <v>43871</v>
+      </c>
+      <c r="F34" s="83">
         <f t="shared" si="33"/>
-        <v>43889</v>
-      </c>
-      <c r="G33" s="58">
+        <v>43875</v>
+      </c>
+      <c r="G34" s="58">
         <v>5</v>
       </c>
-      <c r="H33" s="59">
-        <v>0</v>
-      </c>
-      <c r="I33" s="60">
+      <c r="H34" s="59">
+        <v>1</v>
+      </c>
+      <c r="I34" s="60">
         <f t="shared" si="31"/>
         <v>5</v>
-      </c>
-      <c r="J33" s="79"/>
-      <c r="K33" s="87"/>
-      <c r="L33" s="87"/>
-      <c r="M33" s="87"/>
-      <c r="N33" s="87"/>
-      <c r="O33" s="87"/>
-      <c r="P33" s="87"/>
-      <c r="Q33" s="87"/>
-      <c r="R33" s="87"/>
-      <c r="S33" s="87"/>
-      <c r="T33" s="87"/>
-      <c r="U33" s="87"/>
-      <c r="V33" s="87"/>
-      <c r="W33" s="87"/>
-      <c r="X33" s="87"/>
-      <c r="Y33" s="87"/>
-      <c r="Z33" s="87"/>
-      <c r="AA33" s="87"/>
-      <c r="AB33" s="87"/>
-      <c r="AC33" s="87"/>
-      <c r="AD33" s="87"/>
-      <c r="AE33" s="87"/>
-      <c r="AF33" s="87"/>
-      <c r="AG33" s="87"/>
-      <c r="AH33" s="87"/>
-      <c r="AI33" s="87"/>
-      <c r="AJ33" s="87"/>
-      <c r="AK33" s="87"/>
-      <c r="AL33" s="87"/>
-      <c r="AM33" s="87"/>
-      <c r="AN33" s="87"/>
-      <c r="AO33" s="87"/>
-      <c r="AP33" s="87"/>
-      <c r="AQ33" s="87"/>
-      <c r="AR33" s="87"/>
-      <c r="AS33" s="87"/>
-      <c r="AT33" s="87"/>
-      <c r="AU33" s="87"/>
-      <c r="AV33" s="87"/>
-      <c r="AW33" s="87"/>
-      <c r="AX33" s="87"/>
-      <c r="AY33" s="87"/>
-      <c r="AZ33" s="87"/>
-      <c r="BA33" s="87"/>
-      <c r="BB33" s="87"/>
-      <c r="BC33" s="87"/>
-      <c r="BD33" s="87"/>
-      <c r="BE33" s="87"/>
-      <c r="BF33" s="87"/>
-      <c r="BG33" s="87"/>
-      <c r="BH33" s="87"/>
-      <c r="BI33" s="87"/>
-      <c r="BJ33" s="87"/>
-      <c r="BK33" s="87"/>
-      <c r="BL33" s="87"/>
-      <c r="BM33" s="87"/>
-      <c r="BN33" s="87"/>
-    </row>
-    <row r="34" spans="1:66" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A34" s="56">
-        <v>3.7</v>
-      </c>
-      <c r="B34" s="106" t="s">
-        <v>155</v>
-      </c>
-      <c r="C34" s="57" t="s">
-        <v>143</v>
-      </c>
-      <c r="D34" s="107"/>
-      <c r="E34" s="82">
-        <v>43885</v>
-      </c>
-      <c r="F34" s="83">
-        <f t="shared" si="33"/>
-        <v>43886</v>
-      </c>
-      <c r="G34" s="58">
-        <v>2</v>
-      </c>
-      <c r="H34" s="59">
-        <v>0</v>
-      </c>
-      <c r="I34" s="60">
-        <f t="shared" si="31"/>
-        <v>2</v>
       </c>
       <c r="J34" s="79"/>
       <c r="K34" s="87"/>
@@ -7194,33 +7217,34 @@
       <c r="BM34" s="87"/>
       <c r="BN34" s="87"/>
     </row>
-    <row r="35" spans="1:66" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A35" s="56">
-        <v>3.8</v>
+    <row r="35" spans="1:66" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A35" s="56" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>3.2</v>
       </c>
       <c r="B35" s="106" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C35" s="57" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="D35" s="107"/>
       <c r="E35" s="82">
-        <v>43885</v>
+        <v>43878</v>
       </c>
       <c r="F35" s="83">
         <f t="shared" si="33"/>
-        <v>43887</v>
+        <v>43882</v>
       </c>
       <c r="G35" s="58">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H35" s="59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I35" s="60">
         <f t="shared" si="31"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J35" s="79"/>
       <c r="K35" s="87"/>
@@ -7280,112 +7304,116 @@
       <c r="BM35" s="87"/>
       <c r="BN35" s="87"/>
     </row>
-    <row r="36" spans="1:66" s="51" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A36" s="49" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>4</v>
-      </c>
-      <c r="B36" s="50" t="s">
-        <v>156</v>
-      </c>
-      <c r="D36" s="52"/>
-      <c r="E36" s="84"/>
-      <c r="F36" s="84" t="str">
-        <f t="shared" si="33"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G36" s="53"/>
-      <c r="H36" s="54"/>
-      <c r="I36" s="55" t="str">
+    <row r="36" spans="1:66" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A36" s="56">
+        <v>3.3</v>
+      </c>
+      <c r="B36" s="106" t="s">
+        <v>184</v>
+      </c>
+      <c r="C36" s="57" t="s">
+        <v>139</v>
+      </c>
+      <c r="D36" s="107"/>
+      <c r="E36" s="82">
+        <v>43874</v>
+      </c>
+      <c r="F36" s="83">
+        <v>43875</v>
+      </c>
+      <c r="G36" s="58">
+        <v>2</v>
+      </c>
+      <c r="H36" s="59">
+        <v>1</v>
+      </c>
+      <c r="I36" s="60">
         <f t="shared" si="31"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J36" s="80"/>
-      <c r="K36" s="89"/>
-      <c r="L36" s="89"/>
-      <c r="M36" s="89"/>
-      <c r="N36" s="89"/>
-      <c r="O36" s="89"/>
-      <c r="P36" s="89"/>
-      <c r="Q36" s="89"/>
-      <c r="R36" s="89"/>
-      <c r="S36" s="89"/>
-      <c r="T36" s="89"/>
-      <c r="U36" s="89"/>
-      <c r="V36" s="89"/>
-      <c r="W36" s="89"/>
-      <c r="X36" s="89"/>
-      <c r="Y36" s="89"/>
-      <c r="Z36" s="89"/>
-      <c r="AA36" s="89"/>
-      <c r="AB36" s="89"/>
-      <c r="AC36" s="89"/>
-      <c r="AD36" s="89"/>
-      <c r="AE36" s="89"/>
-      <c r="AF36" s="89"/>
-      <c r="AG36" s="89"/>
-      <c r="AH36" s="89"/>
-      <c r="AI36" s="89"/>
-      <c r="AJ36" s="89"/>
-      <c r="AK36" s="89"/>
-      <c r="AL36" s="89"/>
-      <c r="AM36" s="89"/>
-      <c r="AN36" s="89"/>
-      <c r="AO36" s="89"/>
-      <c r="AP36" s="89"/>
-      <c r="AQ36" s="89"/>
-      <c r="AR36" s="89"/>
-      <c r="AS36" s="89"/>
-      <c r="AT36" s="89"/>
-      <c r="AU36" s="89"/>
-      <c r="AV36" s="89"/>
-      <c r="AW36" s="89"/>
-      <c r="AX36" s="89"/>
-      <c r="AY36" s="89"/>
-      <c r="AZ36" s="89"/>
-      <c r="BA36" s="89"/>
-      <c r="BB36" s="89"/>
-      <c r="BC36" s="89"/>
-      <c r="BD36" s="89"/>
-      <c r="BE36" s="89"/>
-      <c r="BF36" s="89"/>
-      <c r="BG36" s="89"/>
-      <c r="BH36" s="89"/>
-      <c r="BI36" s="89"/>
-      <c r="BJ36" s="89"/>
-      <c r="BK36" s="89"/>
-      <c r="BL36" s="89"/>
-      <c r="BM36" s="89"/>
-      <c r="BN36" s="89"/>
+        <v>2</v>
+      </c>
+      <c r="J36" s="79"/>
+      <c r="K36" s="87"/>
+      <c r="L36" s="87"/>
+      <c r="M36" s="87"/>
+      <c r="N36" s="87"/>
+      <c r="O36" s="87"/>
+      <c r="P36" s="87"/>
+      <c r="Q36" s="87"/>
+      <c r="R36" s="87"/>
+      <c r="S36" s="87"/>
+      <c r="T36" s="87"/>
+      <c r="U36" s="87"/>
+      <c r="V36" s="87"/>
+      <c r="W36" s="87"/>
+      <c r="X36" s="87"/>
+      <c r="Y36" s="87"/>
+      <c r="Z36" s="87"/>
+      <c r="AA36" s="87"/>
+      <c r="AB36" s="87"/>
+      <c r="AC36" s="87"/>
+      <c r="AD36" s="87"/>
+      <c r="AE36" s="87"/>
+      <c r="AF36" s="87"/>
+      <c r="AG36" s="87"/>
+      <c r="AH36" s="87"/>
+      <c r="AI36" s="87"/>
+      <c r="AJ36" s="87"/>
+      <c r="AK36" s="87"/>
+      <c r="AL36" s="87"/>
+      <c r="AM36" s="87"/>
+      <c r="AN36" s="87"/>
+      <c r="AO36" s="87"/>
+      <c r="AP36" s="87"/>
+      <c r="AQ36" s="87"/>
+      <c r="AR36" s="87"/>
+      <c r="AS36" s="87"/>
+      <c r="AT36" s="87"/>
+      <c r="AU36" s="87"/>
+      <c r="AV36" s="87"/>
+      <c r="AW36" s="87"/>
+      <c r="AX36" s="87"/>
+      <c r="AY36" s="87"/>
+      <c r="AZ36" s="87"/>
+      <c r="BA36" s="87"/>
+      <c r="BB36" s="87"/>
+      <c r="BC36" s="87"/>
+      <c r="BD36" s="87"/>
+      <c r="BE36" s="87"/>
+      <c r="BF36" s="87"/>
+      <c r="BG36" s="87"/>
+      <c r="BH36" s="87"/>
+      <c r="BI36" s="87"/>
+      <c r="BJ36" s="87"/>
+      <c r="BK36" s="87"/>
+      <c r="BL36" s="87"/>
+      <c r="BM36" s="87"/>
+      <c r="BN36" s="87"/>
     </row>
     <row r="37" spans="1:66" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A37" s="56" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>4.1</v>
+      <c r="A37" s="56">
+        <v>3.4</v>
       </c>
       <c r="B37" s="106" t="s">
-        <v>164</v>
+        <v>185</v>
       </c>
       <c r="C37" s="57" t="s">
         <v>143</v>
       </c>
       <c r="D37" s="107"/>
       <c r="E37" s="82">
-        <v>43880</v>
+        <v>43881</v>
       </c>
       <c r="F37" s="83">
-        <f t="shared" si="33"/>
         <v>43882</v>
       </c>
       <c r="G37" s="58">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H37" s="59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37" s="60">
-        <f t="shared" si="31"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J37" s="79"/>
       <c r="K37" s="87"/>
@@ -7446,33 +7474,30 @@
       <c r="BN37" s="87"/>
     </row>
     <row r="38" spans="1:66" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A38" s="56" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>4.2</v>
+      <c r="A38" s="56">
+        <v>3.5</v>
       </c>
       <c r="B38" s="106" t="s">
-        <v>165</v>
+        <v>186</v>
       </c>
       <c r="C38" s="57" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="D38" s="107"/>
       <c r="E38" s="82">
-        <v>43899</v>
+        <v>43889</v>
       </c>
       <c r="F38" s="83">
-        <f t="shared" si="33"/>
-        <v>43901</v>
+        <v>43889</v>
       </c>
       <c r="G38" s="58">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H38" s="59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I38" s="60">
-        <f t="shared" si="31"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J38" s="79"/>
       <c r="K38" s="87"/>
@@ -7535,23 +7560,24 @@
     <row r="39" spans="1:66" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A39" s="56" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>4.3</v>
+        <v>3.6</v>
       </c>
       <c r="B39" s="106" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="C39" s="57" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="D39" s="107"/>
       <c r="E39" s="82">
-        <v>43899</v>
+        <v>43885</v>
       </c>
       <c r="F39" s="83">
-        <v>43903</v>
+        <f t="shared" si="33"/>
+        <v>43889</v>
       </c>
       <c r="G39" s="58">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H39" s="59">
         <v>0</v>
@@ -7618,34 +7644,33 @@
       <c r="BM39" s="87"/>
       <c r="BN39" s="87"/>
     </row>
-    <row r="40" spans="1:66" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A40" s="56" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>4.4</v>
+    <row r="40" spans="1:66" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A40" s="56">
+        <v>3.7</v>
       </c>
       <c r="B40" s="106" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="C40" s="57" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D40" s="107"/>
       <c r="E40" s="82">
-        <v>43878</v>
+        <v>43885</v>
       </c>
       <c r="F40" s="83">
         <f t="shared" si="33"/>
-        <v>43882</v>
+        <v>43886</v>
       </c>
       <c r="G40" s="58">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H40" s="59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I40" s="60">
         <f t="shared" si="31"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J40" s="79"/>
       <c r="K40" s="87"/>
@@ -7706,32 +7731,32 @@
       <c r="BN40" s="87"/>
     </row>
     <row r="41" spans="1:66" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A41" s="56" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>4.5</v>
+      <c r="A41" s="56">
+        <v>3.8</v>
       </c>
       <c r="B41" s="106" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="C41" s="57" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D41" s="107"/>
       <c r="E41" s="82">
-        <v>43906</v>
+        <v>43885</v>
       </c>
       <c r="F41" s="83">
-        <v>43910</v>
+        <f t="shared" si="33"/>
+        <v>43887</v>
       </c>
       <c r="G41" s="58">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H41" s="59">
         <v>0</v>
       </c>
       <c r="I41" s="60">
         <f t="shared" si="31"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J41" s="79"/>
       <c r="K41" s="87"/>
@@ -7794,21 +7819,21 @@
     <row r="42" spans="1:66" s="51" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A42" s="49" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B42" s="50" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="D42" s="52"/>
       <c r="E42" s="84"/>
       <c r="F42" s="84" t="str">
-        <f t="shared" ref="F42:F44" si="34">IF(ISBLANK(E42)," - ",IF(G42=0,E42,E42+G42-1))</f>
+        <f t="shared" si="33"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G42" s="53"/>
       <c r="H42" s="54"/>
       <c r="I42" s="55" t="str">
-        <f t="shared" ref="I42:I44" si="35">IF(OR(F42=0,E42=0)," - ",NETWORKDAYS(E42,F42))</f>
+        <f t="shared" si="31"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J42" s="80"/>
@@ -7872,10 +7897,10 @@
     <row r="43" spans="1:66" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A43" s="56" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>5.1</v>
+        <v>4.1</v>
       </c>
       <c r="B43" s="106" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C43" s="57" t="s">
         <v>143</v>
@@ -7885,7 +7910,7 @@
         <v>43880</v>
       </c>
       <c r="F43" s="83">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>43882</v>
       </c>
       <c r="G43" s="58">
@@ -7895,7 +7920,7 @@
         <v>0</v>
       </c>
       <c r="I43" s="60">
-        <f t="shared" si="35"/>
+        <f t="shared" si="31"/>
         <v>3</v>
       </c>
       <c r="J43" s="79"/>
@@ -7959,10 +7984,10 @@
     <row r="44" spans="1:66" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A44" s="56" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>5.2</v>
+        <v>4.2</v>
       </c>
       <c r="B44" s="106" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="C44" s="57" t="s">
         <v>153</v>
@@ -7972,7 +7997,7 @@
         <v>43899</v>
       </c>
       <c r="F44" s="83">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>43901</v>
       </c>
       <c r="G44" s="58">
@@ -7982,7 +8007,7 @@
         <v>0</v>
       </c>
       <c r="I44" s="60">
-        <f t="shared" si="35"/>
+        <f t="shared" si="31"/>
         <v>3</v>
       </c>
       <c r="J44" s="79"/>
@@ -8043,33 +8068,35 @@
       <c r="BM44" s="87"/>
       <c r="BN44" s="87"/>
     </row>
-    <row r="45" spans="1:66" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A45" s="56">
-        <v>5.3</v>
+    <row r="45" spans="1:66" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A45" s="56" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>4.3</v>
       </c>
       <c r="B45" s="106" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
       <c r="C45" s="57" t="s">
         <v>143</v>
       </c>
-      <c r="D45" s="141"/>
-      <c r="E45" s="142">
-        <v>43880</v>
-      </c>
-      <c r="F45" s="143">
-        <v>43880</v>
-      </c>
-      <c r="G45" s="144">
+      <c r="D45" s="107"/>
+      <c r="E45" s="82">
+        <v>43899</v>
+      </c>
+      <c r="F45" s="83">
+        <v>43903</v>
+      </c>
+      <c r="G45" s="58">
         <v>1</v>
       </c>
-      <c r="H45" s="145">
+      <c r="H45" s="59">
         <v>0</v>
       </c>
-      <c r="I45" s="146">
-        <v>1</v>
-      </c>
-      <c r="J45" s="147"/>
+      <c r="I45" s="60">
+        <f t="shared" si="31"/>
+        <v>5</v>
+      </c>
+      <c r="J45" s="79"/>
       <c r="K45" s="87"/>
       <c r="L45" s="87"/>
       <c r="M45" s="87"/>
@@ -8128,32 +8155,35 @@
       <c r="BN45" s="87"/>
     </row>
     <row r="46" spans="1:66" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A46" s="56">
-        <v>5.4</v>
+      <c r="A46" s="56" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>4.4</v>
       </c>
       <c r="B46" s="106" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
       <c r="C46" s="57" t="s">
-        <v>138</v>
-      </c>
-      <c r="D46" s="141"/>
-      <c r="E46" s="142">
-        <v>43885</v>
-      </c>
-      <c r="F46" s="143">
-        <v>43885</v>
-      </c>
-      <c r="G46" s="144">
+        <v>139</v>
+      </c>
+      <c r="D46" s="107"/>
+      <c r="E46" s="82">
+        <v>43878</v>
+      </c>
+      <c r="F46" s="83">
+        <f t="shared" si="33"/>
+        <v>43882</v>
+      </c>
+      <c r="G46" s="58">
+        <v>5</v>
+      </c>
+      <c r="H46" s="59">
         <v>1</v>
       </c>
-      <c r="H46" s="145">
-        <v>0</v>
-      </c>
-      <c r="I46" s="146">
-        <v>1</v>
-      </c>
-      <c r="J46" s="147"/>
+      <c r="I46" s="60">
+        <f t="shared" si="31"/>
+        <v>5</v>
+      </c>
+      <c r="J46" s="79"/>
       <c r="K46" s="87"/>
       <c r="L46" s="87"/>
       <c r="M46" s="87"/>
@@ -8212,32 +8242,34 @@
       <c r="BN46" s="87"/>
     </row>
     <row r="47" spans="1:66" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A47" s="56">
-        <v>5.5</v>
+      <c r="A47" s="56" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>4.5</v>
       </c>
       <c r="B47" s="106" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
       <c r="C47" s="57" t="s">
-        <v>139</v>
-      </c>
-      <c r="D47" s="141"/>
-      <c r="E47" s="142">
-        <v>43899</v>
-      </c>
-      <c r="F47" s="143">
-        <v>43899</v>
-      </c>
-      <c r="G47" s="144">
+        <v>143</v>
+      </c>
+      <c r="D47" s="107"/>
+      <c r="E47" s="82">
+        <v>43906</v>
+      </c>
+      <c r="F47" s="83">
+        <v>43910</v>
+      </c>
+      <c r="G47" s="58">
         <v>1</v>
       </c>
-      <c r="H47" s="145">
+      <c r="H47" s="59">
         <v>0</v>
       </c>
-      <c r="I47" s="146">
-        <v>1</v>
-      </c>
-      <c r="J47" s="147"/>
+      <c r="I47" s="60">
+        <f t="shared" si="31"/>
+        <v>5</v>
+      </c>
+      <c r="J47" s="79"/>
       <c r="K47" s="87"/>
       <c r="L47" s="87"/>
       <c r="M47" s="87"/>
@@ -8295,117 +8327,114 @@
       <c r="BM47" s="87"/>
       <c r="BN47" s="87"/>
     </row>
-    <row r="48" spans="1:66" s="57" customFormat="1" ht="36" x14ac:dyDescent="0.2">
-      <c r="A48" s="56">
-        <v>5.6</v>
-      </c>
-      <c r="B48" s="106" t="s">
-        <v>190</v>
-      </c>
-      <c r="C48" s="57" t="s">
-        <v>138</v>
-      </c>
-      <c r="D48" s="141"/>
-      <c r="E48" s="142">
-        <v>43899</v>
-      </c>
-      <c r="F48" s="143">
-        <v>43899</v>
-      </c>
-      <c r="G48" s="144">
-        <v>1</v>
-      </c>
-      <c r="H48" s="145">
+    <row r="48" spans="1:66" s="51" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A48" s="49" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>5</v>
+      </c>
+      <c r="B48" s="50" t="s">
+        <v>169</v>
+      </c>
+      <c r="D48" s="52"/>
+      <c r="E48" s="84"/>
+      <c r="F48" s="84" t="str">
+        <f t="shared" ref="F48:F50" si="34">IF(ISBLANK(E48)," - ",IF(G48=0,E48,E48+G48-1))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G48" s="53"/>
+      <c r="H48" s="54"/>
+      <c r="I48" s="55" t="str">
+        <f t="shared" ref="I48:I50" si="35">IF(OR(F48=0,E48=0)," - ",NETWORKDAYS(E48,F48))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J48" s="80"/>
+      <c r="K48" s="89"/>
+      <c r="L48" s="89"/>
+      <c r="M48" s="89"/>
+      <c r="N48" s="89"/>
+      <c r="O48" s="89"/>
+      <c r="P48" s="89"/>
+      <c r="Q48" s="89"/>
+      <c r="R48" s="89"/>
+      <c r="S48" s="89"/>
+      <c r="T48" s="89"/>
+      <c r="U48" s="89"/>
+      <c r="V48" s="89"/>
+      <c r="W48" s="89"/>
+      <c r="X48" s="89"/>
+      <c r="Y48" s="89"/>
+      <c r="Z48" s="89"/>
+      <c r="AA48" s="89"/>
+      <c r="AB48" s="89"/>
+      <c r="AC48" s="89"/>
+      <c r="AD48" s="89"/>
+      <c r="AE48" s="89"/>
+      <c r="AF48" s="89"/>
+      <c r="AG48" s="89"/>
+      <c r="AH48" s="89"/>
+      <c r="AI48" s="89"/>
+      <c r="AJ48" s="89"/>
+      <c r="AK48" s="89"/>
+      <c r="AL48" s="89"/>
+      <c r="AM48" s="89"/>
+      <c r="AN48" s="89"/>
+      <c r="AO48" s="89"/>
+      <c r="AP48" s="89"/>
+      <c r="AQ48" s="89"/>
+      <c r="AR48" s="89"/>
+      <c r="AS48" s="89"/>
+      <c r="AT48" s="89"/>
+      <c r="AU48" s="89"/>
+      <c r="AV48" s="89"/>
+      <c r="AW48" s="89"/>
+      <c r="AX48" s="89"/>
+      <c r="AY48" s="89"/>
+      <c r="AZ48" s="89"/>
+      <c r="BA48" s="89"/>
+      <c r="BB48" s="89"/>
+      <c r="BC48" s="89"/>
+      <c r="BD48" s="89"/>
+      <c r="BE48" s="89"/>
+      <c r="BF48" s="89"/>
+      <c r="BG48" s="89"/>
+      <c r="BH48" s="89"/>
+      <c r="BI48" s="89"/>
+      <c r="BJ48" s="89"/>
+      <c r="BK48" s="89"/>
+      <c r="BL48" s="89"/>
+      <c r="BM48" s="89"/>
+      <c r="BN48" s="89"/>
+    </row>
+    <row r="49" spans="1:71" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A49" s="56" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>5.1</v>
+      </c>
+      <c r="B49" s="106" t="s">
+        <v>170</v>
+      </c>
+      <c r="C49" s="57" t="s">
+        <v>143</v>
+      </c>
+      <c r="D49" s="107"/>
+      <c r="E49" s="82">
+        <v>43880</v>
+      </c>
+      <c r="F49" s="83">
+        <f t="shared" si="34"/>
+        <v>43882</v>
+      </c>
+      <c r="G49" s="58">
+        <v>3</v>
+      </c>
+      <c r="H49" s="59">
         <v>0</v>
       </c>
-      <c r="I48" s="146">
-        <v>1</v>
-      </c>
-      <c r="J48" s="147"/>
-      <c r="K48" s="87"/>
-      <c r="L48" s="87"/>
-      <c r="M48" s="87"/>
-      <c r="N48" s="87"/>
-      <c r="O48" s="87"/>
-      <c r="P48" s="87"/>
-      <c r="Q48" s="87"/>
-      <c r="R48" s="87"/>
-      <c r="S48" s="87"/>
-      <c r="T48" s="87"/>
-      <c r="U48" s="87"/>
-      <c r="V48" s="87"/>
-      <c r="W48" s="87"/>
-      <c r="X48" s="87"/>
-      <c r="Y48" s="87"/>
-      <c r="Z48" s="87"/>
-      <c r="AA48" s="87"/>
-      <c r="AB48" s="87"/>
-      <c r="AC48" s="87"/>
-      <c r="AD48" s="87"/>
-      <c r="AE48" s="87"/>
-      <c r="AF48" s="87"/>
-      <c r="AG48" s="87"/>
-      <c r="AH48" s="87"/>
-      <c r="AI48" s="87"/>
-      <c r="AJ48" s="87"/>
-      <c r="AK48" s="87"/>
-      <c r="AL48" s="87"/>
-      <c r="AM48" s="87"/>
-      <c r="AN48" s="87"/>
-      <c r="AO48" s="87"/>
-      <c r="AP48" s="87"/>
-      <c r="AQ48" s="87"/>
-      <c r="AR48" s="87"/>
-      <c r="AS48" s="87"/>
-      <c r="AT48" s="87"/>
-      <c r="AU48" s="87"/>
-      <c r="AV48" s="87"/>
-      <c r="AW48" s="87"/>
-      <c r="AX48" s="87"/>
-      <c r="AY48" s="87"/>
-      <c r="AZ48" s="87"/>
-      <c r="BA48" s="87"/>
-      <c r="BB48" s="87"/>
-      <c r="BC48" s="87"/>
-      <c r="BD48" s="87"/>
-      <c r="BE48" s="87"/>
-      <c r="BF48" s="87"/>
-      <c r="BG48" s="87"/>
-      <c r="BH48" s="87"/>
-      <c r="BI48" s="87"/>
-      <c r="BJ48" s="87"/>
-      <c r="BK48" s="87"/>
-      <c r="BL48" s="87"/>
-      <c r="BM48" s="87"/>
-      <c r="BN48" s="87"/>
-    </row>
-    <row r="49" spans="1:71" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A49" s="56">
-        <v>5.7</v>
-      </c>
-      <c r="B49" s="106" t="s">
-        <v>191</v>
-      </c>
-      <c r="C49" s="57" t="s">
-        <v>139</v>
-      </c>
-      <c r="D49" s="141"/>
-      <c r="E49" s="142">
-        <v>43906</v>
-      </c>
-      <c r="F49" s="143">
-        <v>43906</v>
-      </c>
-      <c r="G49" s="144">
-        <v>1</v>
-      </c>
-      <c r="H49" s="145">
-        <v>0</v>
-      </c>
-      <c r="I49" s="146">
-        <v>1</v>
-      </c>
-      <c r="J49" s="147"/>
+      <c r="I49" s="60">
+        <f t="shared" si="35"/>
+        <v>3</v>
+      </c>
+      <c r="J49" s="79"/>
       <c r="K49" s="87"/>
       <c r="L49" s="87"/>
       <c r="M49" s="87"/>
@@ -8464,32 +8493,35 @@
       <c r="BN49" s="87"/>
     </row>
     <row r="50" spans="1:71" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A50" s="56">
-        <v>5.8</v>
+      <c r="A50" s="56" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>5.2</v>
       </c>
       <c r="B50" s="106" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
       <c r="C50" s="57" t="s">
-        <v>138</v>
-      </c>
-      <c r="D50" s="141"/>
-      <c r="E50" s="142">
-        <v>43906</v>
-      </c>
-      <c r="F50" s="143">
-        <v>43906</v>
-      </c>
-      <c r="G50" s="144">
-        <v>1</v>
-      </c>
-      <c r="H50" s="145">
+        <v>153</v>
+      </c>
+      <c r="D50" s="107"/>
+      <c r="E50" s="82">
+        <v>43899</v>
+      </c>
+      <c r="F50" s="83">
+        <f t="shared" si="34"/>
+        <v>43901</v>
+      </c>
+      <c r="G50" s="58">
+        <v>3</v>
+      </c>
+      <c r="H50" s="59">
         <v>0</v>
       </c>
-      <c r="I50" s="146">
-        <v>1</v>
-      </c>
-      <c r="J50" s="147"/>
+      <c r="I50" s="60">
+        <f t="shared" si="35"/>
+        <v>3</v>
+      </c>
+      <c r="J50" s="79"/>
       <c r="K50" s="87"/>
       <c r="L50" s="87"/>
       <c r="M50" s="87"/>
@@ -8547,28 +8579,28 @@
       <c r="BM50" s="87"/>
       <c r="BN50" s="87"/>
     </row>
-    <row r="51" spans="1:71" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:71" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A51" s="56">
-        <v>5.9</v>
+        <v>5.3</v>
       </c>
       <c r="B51" s="106" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="C51" s="57" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="D51" s="141"/>
       <c r="E51" s="142">
-        <v>43913</v>
+        <v>43880</v>
       </c>
       <c r="F51" s="143">
-        <v>43913</v>
+        <v>43880</v>
       </c>
       <c r="G51" s="144">
         <v>1</v>
       </c>
       <c r="H51" s="145">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I51" s="146">
         <v>1</v>
@@ -8631,112 +8663,117 @@
       <c r="BM51" s="87"/>
       <c r="BN51" s="87"/>
     </row>
-    <row r="52" spans="1:71" s="51" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A52" s="49" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>6</v>
-      </c>
-      <c r="B52" s="50" t="s">
-        <v>194</v>
-      </c>
-      <c r="D52" s="52"/>
-      <c r="E52" s="84"/>
-      <c r="F52" s="84" t="str">
-        <f t="shared" ref="F52" si="36">IF(ISBLANK(E52)," - ",IF(G52=0,E52,E52+G52-1))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G52" s="53"/>
-      <c r="H52" s="54"/>
-      <c r="I52" s="55" t="str">
-        <f t="shared" ref="I52:I53" si="37">IF(OR(F52=0,E52=0)," - ",NETWORKDAYS(E52,F52))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J52" s="80"/>
-      <c r="K52" s="89"/>
-      <c r="L52" s="89"/>
-      <c r="M52" s="89"/>
-      <c r="N52" s="89"/>
-      <c r="O52" s="89"/>
-      <c r="P52" s="89"/>
-      <c r="Q52" s="89"/>
-      <c r="R52" s="89"/>
-      <c r="S52" s="89"/>
-      <c r="T52" s="89"/>
-      <c r="U52" s="89"/>
-      <c r="V52" s="89"/>
-      <c r="W52" s="89"/>
-      <c r="X52" s="89"/>
-      <c r="Y52" s="89"/>
-      <c r="Z52" s="89"/>
-      <c r="AA52" s="89"/>
-      <c r="AB52" s="89"/>
-      <c r="AC52" s="89"/>
-      <c r="AD52" s="89"/>
-      <c r="AE52" s="89"/>
-      <c r="AF52" s="89"/>
-      <c r="AG52" s="89"/>
-      <c r="AH52" s="89"/>
-      <c r="AI52" s="89"/>
-      <c r="AJ52" s="89"/>
-      <c r="AK52" s="89"/>
-      <c r="AL52" s="89"/>
-      <c r="AM52" s="89"/>
-      <c r="AN52" s="89"/>
-      <c r="AO52" s="89"/>
-      <c r="AP52" s="89"/>
-      <c r="AQ52" s="89"/>
-      <c r="AR52" s="89"/>
-      <c r="AS52" s="89"/>
-      <c r="AT52" s="89"/>
-      <c r="AU52" s="89"/>
-      <c r="AV52" s="89"/>
-      <c r="AW52" s="89"/>
-      <c r="AX52" s="89"/>
-      <c r="AY52" s="89"/>
-      <c r="AZ52" s="89"/>
-      <c r="BA52" s="89"/>
-      <c r="BB52" s="89"/>
-      <c r="BC52" s="89"/>
-      <c r="BD52" s="89"/>
-      <c r="BE52" s="89"/>
-      <c r="BF52" s="89"/>
-      <c r="BG52" s="89"/>
-      <c r="BH52" s="89"/>
-      <c r="BI52" s="89"/>
-      <c r="BJ52" s="89"/>
-      <c r="BK52" s="89"/>
-      <c r="BL52" s="89"/>
-      <c r="BM52" s="89"/>
-      <c r="BN52" s="89"/>
-    </row>
-    <row r="53" spans="1:71" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:71" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A52" s="56">
+        <v>5.4</v>
+      </c>
+      <c r="B52" s="106" t="s">
+        <v>188</v>
+      </c>
+      <c r="C52" s="57" t="s">
+        <v>138</v>
+      </c>
+      <c r="D52" s="141"/>
+      <c r="E52" s="142">
+        <v>43885</v>
+      </c>
+      <c r="F52" s="143">
+        <v>43885</v>
+      </c>
+      <c r="G52" s="144">
+        <v>1</v>
+      </c>
+      <c r="H52" s="145">
+        <v>1</v>
+      </c>
+      <c r="I52" s="146">
+        <v>1</v>
+      </c>
+      <c r="J52" s="147"/>
+      <c r="K52" s="87"/>
+      <c r="L52" s="87"/>
+      <c r="M52" s="87"/>
+      <c r="N52" s="87"/>
+      <c r="O52" s="87"/>
+      <c r="P52" s="87"/>
+      <c r="Q52" s="87"/>
+      <c r="R52" s="87"/>
+      <c r="S52" s="87"/>
+      <c r="T52" s="87"/>
+      <c r="U52" s="87"/>
+      <c r="V52" s="87"/>
+      <c r="W52" s="87"/>
+      <c r="X52" s="87"/>
+      <c r="Y52" s="87"/>
+      <c r="Z52" s="87"/>
+      <c r="AA52" s="87"/>
+      <c r="AB52" s="87"/>
+      <c r="AC52" s="87"/>
+      <c r="AD52" s="87"/>
+      <c r="AE52" s="87"/>
+      <c r="AF52" s="87"/>
+      <c r="AG52" s="87"/>
+      <c r="AH52" s="87"/>
+      <c r="AI52" s="87"/>
+      <c r="AJ52" s="87"/>
+      <c r="AK52" s="87"/>
+      <c r="AL52" s="87"/>
+      <c r="AM52" s="87"/>
+      <c r="AN52" s="87"/>
+      <c r="AO52" s="87"/>
+      <c r="AP52" s="87"/>
+      <c r="AQ52" s="87"/>
+      <c r="AR52" s="87"/>
+      <c r="AS52" s="87"/>
+      <c r="AT52" s="87"/>
+      <c r="AU52" s="87"/>
+      <c r="AV52" s="87"/>
+      <c r="AW52" s="87"/>
+      <c r="AX52" s="87"/>
+      <c r="AY52" s="87"/>
+      <c r="AZ52" s="87"/>
+      <c r="BA52" s="87"/>
+      <c r="BB52" s="87"/>
+      <c r="BC52" s="87"/>
+      <c r="BD52" s="87"/>
+      <c r="BE52" s="87"/>
+      <c r="BF52" s="87"/>
+      <c r="BG52" s="87"/>
+      <c r="BH52" s="87"/>
+      <c r="BI52" s="87"/>
+      <c r="BJ52" s="87"/>
+      <c r="BK52" s="87"/>
+      <c r="BL52" s="87"/>
+      <c r="BM52" s="87"/>
+      <c r="BN52" s="87"/>
+    </row>
+    <row r="53" spans="1:71" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A53" s="56">
-        <v>6.1</v>
+        <v>5.5</v>
       </c>
       <c r="B53" s="106" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="C53" s="57" t="s">
-        <v>163</v>
-      </c>
-      <c r="D53" s="107"/>
-      <c r="E53" s="82">
-        <v>43913</v>
-      </c>
-      <c r="F53" s="83">
-        <v>43917</v>
-      </c>
-      <c r="G53" s="58">
-        <v>2</v>
-      </c>
-      <c r="H53" s="59">
+        <v>139</v>
+      </c>
+      <c r="D53" s="141"/>
+      <c r="E53" s="142">
+        <v>43899</v>
+      </c>
+      <c r="F53" s="143">
+        <v>43899</v>
+      </c>
+      <c r="G53" s="144">
+        <v>1</v>
+      </c>
+      <c r="H53" s="145">
         <v>0</v>
       </c>
-      <c r="I53" s="60">
-        <f t="shared" si="37"/>
-        <v>5</v>
-      </c>
-      <c r="J53" s="79"/>
+      <c r="I53" s="146">
+        <v>1</v>
+      </c>
+      <c r="J53" s="147"/>
       <c r="K53" s="87"/>
       <c r="L53" s="87"/>
       <c r="M53" s="87"/>
@@ -8793,37 +8830,32 @@
       <c r="BL53" s="87"/>
       <c r="BM53" s="87"/>
       <c r="BN53" s="87"/>
-      <c r="BO53" s="149"/>
-      <c r="BP53" s="149"/>
-      <c r="BQ53" s="149"/>
-      <c r="BR53" s="149"/>
-      <c r="BS53" s="149"/>
-    </row>
-    <row r="54" spans="1:71" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:71" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A54" s="56">
-        <v>6.2</v>
+        <v>5.6</v>
       </c>
       <c r="B54" s="106" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="C54" s="57" t="s">
-        <v>163</v>
+        <v>138</v>
       </c>
       <c r="D54" s="141"/>
       <c r="E54" s="142">
-        <v>43920</v>
+        <v>43899</v>
       </c>
       <c r="F54" s="143">
-        <v>43924</v>
+        <v>43899</v>
       </c>
       <c r="G54" s="144">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H54" s="145">
         <v>0</v>
       </c>
       <c r="I54" s="146">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J54" s="147"/>
       <c r="K54" s="87"/>
@@ -8882,118 +8914,118 @@
       <c r="BL54" s="87"/>
       <c r="BM54" s="87"/>
       <c r="BN54" s="87"/>
-      <c r="BO54" s="149"/>
-      <c r="BP54" s="149"/>
-      <c r="BQ54" s="149"/>
-      <c r="BR54" s="149"/>
-      <c r="BS54" s="149"/>
-    </row>
-    <row r="55" spans="1:71" s="51" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A55" s="49" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>7</v>
-      </c>
-      <c r="B55" s="50" t="s">
-        <v>172</v>
-      </c>
-      <c r="D55" s="52"/>
-      <c r="E55" s="84"/>
-      <c r="F55" s="84" t="str">
-        <f t="shared" ref="F55" si="38">IF(ISBLANK(E55)," - ",IF(G55=0,E55,E55+G55-1))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G55" s="53"/>
-      <c r="H55" s="54"/>
-      <c r="I55" s="55" t="str">
-        <f t="shared" ref="I55:I61" si="39">IF(OR(F55=0,E55=0)," - ",NETWORKDAYS(E55,F55))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J55" s="80"/>
-      <c r="K55" s="89"/>
-      <c r="L55" s="89"/>
-      <c r="M55" s="89"/>
-      <c r="N55" s="89"/>
-      <c r="O55" s="89"/>
-      <c r="P55" s="89"/>
-      <c r="Q55" s="89"/>
-      <c r="R55" s="89"/>
-      <c r="S55" s="89"/>
-      <c r="T55" s="89"/>
-      <c r="U55" s="89"/>
-      <c r="V55" s="89"/>
-      <c r="W55" s="89"/>
-      <c r="X55" s="89"/>
-      <c r="Y55" s="89"/>
-      <c r="Z55" s="89"/>
-      <c r="AA55" s="89"/>
-      <c r="AB55" s="89"/>
-      <c r="AC55" s="89"/>
-      <c r="AD55" s="89"/>
-      <c r="AE55" s="89"/>
-      <c r="AF55" s="89"/>
-      <c r="AG55" s="89"/>
-      <c r="AH55" s="89"/>
-      <c r="AI55" s="89"/>
-      <c r="AJ55" s="89"/>
-      <c r="AK55" s="89"/>
-      <c r="AL55" s="89"/>
-      <c r="AM55" s="89"/>
-      <c r="AN55" s="89"/>
-      <c r="AO55" s="89"/>
-      <c r="AP55" s="89"/>
-      <c r="AQ55" s="89"/>
-      <c r="AR55" s="89"/>
-      <c r="AS55" s="89"/>
-      <c r="AT55" s="89"/>
-      <c r="AU55" s="89"/>
-      <c r="AV55" s="89"/>
-      <c r="AW55" s="89"/>
-      <c r="AX55" s="89"/>
-      <c r="AY55" s="89"/>
-      <c r="AZ55" s="89"/>
-      <c r="BA55" s="89"/>
-      <c r="BB55" s="89"/>
-      <c r="BC55" s="89"/>
-      <c r="BD55" s="89"/>
-      <c r="BE55" s="89"/>
-      <c r="BF55" s="89"/>
-      <c r="BG55" s="89"/>
-      <c r="BH55" s="89"/>
-      <c r="BI55" s="89"/>
-      <c r="BJ55" s="89"/>
-      <c r="BK55" s="89"/>
-      <c r="BL55" s="89"/>
-      <c r="BM55" s="89"/>
-      <c r="BN55" s="89"/>
+    </row>
+    <row r="55" spans="1:71" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A55" s="56">
+        <v>5.7</v>
+      </c>
+      <c r="B55" s="106" t="s">
+        <v>190</v>
+      </c>
+      <c r="C55" s="57" t="s">
+        <v>139</v>
+      </c>
+      <c r="D55" s="141"/>
+      <c r="E55" s="142">
+        <v>43906</v>
+      </c>
+      <c r="F55" s="143">
+        <v>43906</v>
+      </c>
+      <c r="G55" s="144">
+        <v>1</v>
+      </c>
+      <c r="H55" s="145">
+        <v>0</v>
+      </c>
+      <c r="I55" s="146">
+        <v>1</v>
+      </c>
+      <c r="J55" s="147"/>
+      <c r="K55" s="87"/>
+      <c r="L55" s="87"/>
+      <c r="M55" s="87"/>
+      <c r="N55" s="87"/>
+      <c r="O55" s="87"/>
+      <c r="P55" s="87"/>
+      <c r="Q55" s="87"/>
+      <c r="R55" s="87"/>
+      <c r="S55" s="87"/>
+      <c r="T55" s="87"/>
+      <c r="U55" s="87"/>
+      <c r="V55" s="87"/>
+      <c r="W55" s="87"/>
+      <c r="X55" s="87"/>
+      <c r="Y55" s="87"/>
+      <c r="Z55" s="87"/>
+      <c r="AA55" s="87"/>
+      <c r="AB55" s="87"/>
+      <c r="AC55" s="87"/>
+      <c r="AD55" s="87"/>
+      <c r="AE55" s="87"/>
+      <c r="AF55" s="87"/>
+      <c r="AG55" s="87"/>
+      <c r="AH55" s="87"/>
+      <c r="AI55" s="87"/>
+      <c r="AJ55" s="87"/>
+      <c r="AK55" s="87"/>
+      <c r="AL55" s="87"/>
+      <c r="AM55" s="87"/>
+      <c r="AN55" s="87"/>
+      <c r="AO55" s="87"/>
+      <c r="AP55" s="87"/>
+      <c r="AQ55" s="87"/>
+      <c r="AR55" s="87"/>
+      <c r="AS55" s="87"/>
+      <c r="AT55" s="87"/>
+      <c r="AU55" s="87"/>
+      <c r="AV55" s="87"/>
+      <c r="AW55" s="87"/>
+      <c r="AX55" s="87"/>
+      <c r="AY55" s="87"/>
+      <c r="AZ55" s="87"/>
+      <c r="BA55" s="87"/>
+      <c r="BB55" s="87"/>
+      <c r="BC55" s="87"/>
+      <c r="BD55" s="87"/>
+      <c r="BE55" s="87"/>
+      <c r="BF55" s="87"/>
+      <c r="BG55" s="87"/>
+      <c r="BH55" s="87"/>
+      <c r="BI55" s="87"/>
+      <c r="BJ55" s="87"/>
+      <c r="BK55" s="87"/>
+      <c r="BL55" s="87"/>
+      <c r="BM55" s="87"/>
+      <c r="BN55" s="87"/>
     </row>
     <row r="56" spans="1:71" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A56" s="56">
-        <v>7.1</v>
+        <v>5.8</v>
       </c>
       <c r="B56" s="106" t="s">
-        <v>173</v>
+        <v>191</v>
       </c>
       <c r="C56" s="57" t="s">
-        <v>139</v>
-      </c>
-      <c r="D56" s="107"/>
-      <c r="E56" s="82">
-        <v>43927</v>
-      </c>
-      <c r="F56" s="83">
-        <v>43931</v>
-      </c>
-      <c r="G56" s="58">
-        <v>2</v>
-      </c>
-      <c r="H56" s="59">
+        <v>138</v>
+      </c>
+      <c r="D56" s="141"/>
+      <c r="E56" s="142">
+        <v>43906</v>
+      </c>
+      <c r="F56" s="143">
+        <v>43906</v>
+      </c>
+      <c r="G56" s="144">
+        <v>1</v>
+      </c>
+      <c r="H56" s="145">
         <v>0</v>
       </c>
-      <c r="I56" s="60">
-        <f t="shared" si="39"/>
-        <v>5</v>
-      </c>
-      <c r="J56" s="79"/>
+      <c r="I56" s="146">
+        <v>1</v>
+      </c>
+      <c r="J56" s="147"/>
       <c r="K56" s="87"/>
       <c r="L56" s="87"/>
       <c r="M56" s="87"/>
@@ -9050,40 +9082,34 @@
       <c r="BL56" s="87"/>
       <c r="BM56" s="87"/>
       <c r="BN56" s="87"/>
-      <c r="BO56" s="148"/>
-      <c r="BP56" s="148"/>
-      <c r="BQ56" s="148"/>
-      <c r="BR56" s="148"/>
-      <c r="BS56" s="148"/>
-    </row>
-    <row r="57" spans="1:71" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="1:71" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A57" s="56">
-        <v>7.2</v>
+        <v>5.9</v>
       </c>
       <c r="B57" s="106" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="C57" s="57" t="s">
-        <v>139</v>
-      </c>
-      <c r="D57" s="107"/>
-      <c r="E57" s="82">
-        <v>43927</v>
-      </c>
-      <c r="F57" s="83">
-        <v>43931</v>
-      </c>
-      <c r="G57" s="58">
-        <v>2</v>
-      </c>
-      <c r="H57" s="59">
+        <v>138</v>
+      </c>
+      <c r="D57" s="141"/>
+      <c r="E57" s="142">
+        <v>43913</v>
+      </c>
+      <c r="F57" s="143">
+        <v>43913</v>
+      </c>
+      <c r="G57" s="144">
+        <v>1</v>
+      </c>
+      <c r="H57" s="145">
         <v>0</v>
       </c>
-      <c r="I57" s="60">
-        <f t="shared" si="39"/>
-        <v>5</v>
-      </c>
-      <c r="J57" s="79"/>
+      <c r="I57" s="146">
+        <v>1</v>
+      </c>
+      <c r="J57" s="147"/>
       <c r="K57" s="87"/>
       <c r="L57" s="87"/>
       <c r="M57" s="87"/>
@@ -9140,118 +9166,101 @@
       <c r="BL57" s="87"/>
       <c r="BM57" s="87"/>
       <c r="BN57" s="87"/>
-      <c r="BO57" s="148"/>
-      <c r="BP57" s="148"/>
-      <c r="BQ57" s="148"/>
-      <c r="BR57" s="148"/>
-      <c r="BS57" s="148"/>
-    </row>
-    <row r="58" spans="1:71" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A58" s="56">
-        <v>7.3</v>
-      </c>
-      <c r="B58" s="106" t="s">
-        <v>175</v>
-      </c>
-      <c r="C58" s="57" t="s">
-        <v>138</v>
-      </c>
-      <c r="D58" s="107"/>
-      <c r="E58" s="82">
-        <v>43927</v>
-      </c>
-      <c r="F58" s="83">
-        <v>43931</v>
-      </c>
-      <c r="G58" s="58">
-        <v>2</v>
-      </c>
-      <c r="H58" s="59">
-        <v>0</v>
-      </c>
-      <c r="I58" s="60">
-        <f t="shared" si="39"/>
-        <v>5</v>
-      </c>
-      <c r="J58" s="79"/>
-      <c r="K58" s="87"/>
-      <c r="L58" s="87"/>
-      <c r="M58" s="87"/>
-      <c r="N58" s="87"/>
-      <c r="O58" s="87"/>
-      <c r="P58" s="87"/>
-      <c r="Q58" s="87"/>
-      <c r="R58" s="87"/>
-      <c r="S58" s="87"/>
-      <c r="T58" s="87"/>
-      <c r="U58" s="87"/>
-      <c r="V58" s="87"/>
-      <c r="W58" s="87"/>
-      <c r="X58" s="87"/>
-      <c r="Y58" s="87"/>
-      <c r="Z58" s="87"/>
-      <c r="AA58" s="87"/>
-      <c r="AB58" s="87"/>
-      <c r="AC58" s="87"/>
-      <c r="AD58" s="87"/>
-      <c r="AE58" s="87"/>
-      <c r="AF58" s="87"/>
-      <c r="AG58" s="87"/>
-      <c r="AH58" s="87"/>
-      <c r="AI58" s="87"/>
-      <c r="AJ58" s="87"/>
-      <c r="AK58" s="87"/>
-      <c r="AL58" s="87"/>
-      <c r="AM58" s="87"/>
-      <c r="AN58" s="87"/>
-      <c r="AO58" s="87"/>
-      <c r="AP58" s="87"/>
-      <c r="AQ58" s="87"/>
-      <c r="AR58" s="87"/>
-      <c r="AS58" s="87"/>
-      <c r="AT58" s="87"/>
-      <c r="AU58" s="87"/>
-      <c r="AV58" s="87"/>
-      <c r="AW58" s="87"/>
-      <c r="AX58" s="87"/>
-      <c r="AY58" s="87"/>
-      <c r="AZ58" s="87"/>
-      <c r="BA58" s="87"/>
-      <c r="BB58" s="87"/>
-      <c r="BC58" s="87"/>
-      <c r="BD58" s="87"/>
-      <c r="BE58" s="87"/>
-      <c r="BF58" s="87"/>
-      <c r="BG58" s="87"/>
-      <c r="BH58" s="87"/>
-      <c r="BI58" s="87"/>
-      <c r="BJ58" s="87"/>
-      <c r="BK58" s="87"/>
-      <c r="BL58" s="87"/>
-      <c r="BM58" s="87"/>
-      <c r="BN58" s="87"/>
-      <c r="BO58" s="148"/>
-      <c r="BP58" s="148"/>
-      <c r="BQ58" s="148"/>
-      <c r="BR58" s="148"/>
-      <c r="BS58" s="148"/>
-    </row>
-    <row r="59" spans="1:71" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:71" s="51" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A58" s="49" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>6</v>
+      </c>
+      <c r="B58" s="50" t="s">
+        <v>193</v>
+      </c>
+      <c r="D58" s="52"/>
+      <c r="E58" s="84"/>
+      <c r="F58" s="84" t="str">
+        <f t="shared" ref="F58" si="36">IF(ISBLANK(E58)," - ",IF(G58=0,E58,E58+G58-1))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G58" s="53"/>
+      <c r="H58" s="54"/>
+      <c r="I58" s="55" t="str">
+        <f t="shared" ref="I58:I59" si="37">IF(OR(F58=0,E58=0)," - ",NETWORKDAYS(E58,F58))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J58" s="80"/>
+      <c r="K58" s="89"/>
+      <c r="L58" s="89"/>
+      <c r="M58" s="89"/>
+      <c r="N58" s="89"/>
+      <c r="O58" s="89"/>
+      <c r="P58" s="89"/>
+      <c r="Q58" s="89"/>
+      <c r="R58" s="89"/>
+      <c r="S58" s="89"/>
+      <c r="T58" s="89"/>
+      <c r="U58" s="89"/>
+      <c r="V58" s="89"/>
+      <c r="W58" s="89"/>
+      <c r="X58" s="89"/>
+      <c r="Y58" s="89"/>
+      <c r="Z58" s="89"/>
+      <c r="AA58" s="89"/>
+      <c r="AB58" s="89"/>
+      <c r="AC58" s="89"/>
+      <c r="AD58" s="89"/>
+      <c r="AE58" s="89"/>
+      <c r="AF58" s="89"/>
+      <c r="AG58" s="89"/>
+      <c r="AH58" s="89"/>
+      <c r="AI58" s="89"/>
+      <c r="AJ58" s="89"/>
+      <c r="AK58" s="89"/>
+      <c r="AL58" s="89"/>
+      <c r="AM58" s="89"/>
+      <c r="AN58" s="89"/>
+      <c r="AO58" s="89"/>
+      <c r="AP58" s="89"/>
+      <c r="AQ58" s="89"/>
+      <c r="AR58" s="89"/>
+      <c r="AS58" s="89"/>
+      <c r="AT58" s="89"/>
+      <c r="AU58" s="89"/>
+      <c r="AV58" s="89"/>
+      <c r="AW58" s="89"/>
+      <c r="AX58" s="89"/>
+      <c r="AY58" s="89"/>
+      <c r="AZ58" s="89"/>
+      <c r="BA58" s="89"/>
+      <c r="BB58" s="89"/>
+      <c r="BC58" s="89"/>
+      <c r="BD58" s="89"/>
+      <c r="BE58" s="89"/>
+      <c r="BF58" s="89"/>
+      <c r="BG58" s="89"/>
+      <c r="BH58" s="89"/>
+      <c r="BI58" s="89"/>
+      <c r="BJ58" s="89"/>
+      <c r="BK58" s="89"/>
+      <c r="BL58" s="89"/>
+      <c r="BM58" s="89"/>
+      <c r="BN58" s="89"/>
+    </row>
+    <row r="59" spans="1:71" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A59" s="56">
-        <v>7.4</v>
+        <v>6.1</v>
       </c>
       <c r="B59" s="106" t="s">
-        <v>176</v>
+        <v>194</v>
       </c>
       <c r="C59" s="57" t="s">
-        <v>138</v>
+        <v>163</v>
       </c>
       <c r="D59" s="107"/>
       <c r="E59" s="82">
-        <v>43927</v>
+        <v>43913</v>
       </c>
       <c r="F59" s="83">
-        <v>43931</v>
+        <v>43917</v>
       </c>
       <c r="G59" s="58">
         <v>2</v>
@@ -9260,7 +9269,7 @@
         <v>0</v>
       </c>
       <c r="I59" s="60">
-        <f t="shared" si="39"/>
+        <f t="shared" si="37"/>
         <v>5</v>
       </c>
       <c r="J59" s="79"/>
@@ -9320,40 +9329,39 @@
       <c r="BL59" s="87"/>
       <c r="BM59" s="87"/>
       <c r="BN59" s="87"/>
-      <c r="BO59" s="148"/>
-      <c r="BP59" s="148"/>
-      <c r="BQ59" s="148"/>
-      <c r="BR59" s="148"/>
-      <c r="BS59" s="148"/>
-    </row>
-    <row r="60" spans="1:71" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="BO59" s="149"/>
+      <c r="BP59" s="149"/>
+      <c r="BQ59" s="149"/>
+      <c r="BR59" s="149"/>
+      <c r="BS59" s="149"/>
+    </row>
+    <row r="60" spans="1:71" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A60" s="56">
-        <v>7.5</v>
+        <v>6.2</v>
       </c>
       <c r="B60" s="106" t="s">
-        <v>177</v>
+        <v>195</v>
       </c>
       <c r="C60" s="57" t="s">
-        <v>143</v>
-      </c>
-      <c r="D60" s="107"/>
-      <c r="E60" s="82">
-        <v>43927</v>
-      </c>
-      <c r="F60" s="83">
-        <v>43931</v>
-      </c>
-      <c r="G60" s="58">
+        <v>163</v>
+      </c>
+      <c r="D60" s="141"/>
+      <c r="E60" s="142">
+        <v>43920</v>
+      </c>
+      <c r="F60" s="143">
+        <v>43924</v>
+      </c>
+      <c r="G60" s="144">
         <v>2</v>
       </c>
-      <c r="H60" s="59">
+      <c r="H60" s="145">
         <v>0</v>
       </c>
-      <c r="I60" s="60">
-        <f t="shared" si="39"/>
+      <c r="I60" s="146">
         <v>5</v>
       </c>
-      <c r="J60" s="79"/>
+      <c r="J60" s="147"/>
       <c r="K60" s="87"/>
       <c r="L60" s="87"/>
       <c r="M60" s="87"/>
@@ -9410,126 +9418,115 @@
       <c r="BL60" s="87"/>
       <c r="BM60" s="87"/>
       <c r="BN60" s="87"/>
-      <c r="BO60" s="148"/>
-      <c r="BP60" s="148"/>
-      <c r="BQ60" s="148"/>
-      <c r="BR60" s="148"/>
-      <c r="BS60" s="148"/>
-    </row>
-    <row r="61" spans="1:71" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A61" s="56">
-        <v>7.6</v>
-      </c>
-      <c r="B61" s="106" t="s">
-        <v>178</v>
-      </c>
-      <c r="C61" s="57" t="s">
-        <v>143</v>
-      </c>
-      <c r="D61" s="107"/>
-      <c r="E61" s="82">
-        <v>43927</v>
-      </c>
-      <c r="F61" s="83">
-        <v>43931</v>
-      </c>
-      <c r="G61" s="58">
-        <v>2</v>
-      </c>
-      <c r="H61" s="59">
-        <v>0</v>
-      </c>
-      <c r="I61" s="60">
-        <f t="shared" si="39"/>
-        <v>5</v>
-      </c>
-      <c r="J61" s="79"/>
-      <c r="K61" s="87"/>
-      <c r="L61" s="87"/>
-      <c r="M61" s="87"/>
-      <c r="N61" s="87"/>
-      <c r="O61" s="87"/>
-      <c r="P61" s="87"/>
-      <c r="Q61" s="87"/>
-      <c r="R61" s="87"/>
-      <c r="S61" s="87"/>
-      <c r="T61" s="87"/>
-      <c r="U61" s="87"/>
-      <c r="V61" s="87"/>
-      <c r="W61" s="87"/>
-      <c r="X61" s="87"/>
-      <c r="Y61" s="87"/>
-      <c r="Z61" s="87"/>
-      <c r="AA61" s="87"/>
-      <c r="AB61" s="87"/>
-      <c r="AC61" s="87"/>
-      <c r="AD61" s="87"/>
-      <c r="AE61" s="87"/>
-      <c r="AF61" s="87"/>
-      <c r="AG61" s="87"/>
-      <c r="AH61" s="87"/>
-      <c r="AI61" s="87"/>
-      <c r="AJ61" s="87"/>
-      <c r="AK61" s="87"/>
-      <c r="AL61" s="87"/>
-      <c r="AM61" s="87"/>
-      <c r="AN61" s="87"/>
-      <c r="AO61" s="87"/>
-      <c r="AP61" s="87"/>
-      <c r="AQ61" s="87"/>
-      <c r="AR61" s="87"/>
-      <c r="AS61" s="87"/>
-      <c r="AT61" s="87"/>
-      <c r="AU61" s="87"/>
-      <c r="AV61" s="87"/>
-      <c r="AW61" s="87"/>
-      <c r="AX61" s="87"/>
-      <c r="AY61" s="87"/>
-      <c r="AZ61" s="87"/>
-      <c r="BA61" s="87"/>
-      <c r="BB61" s="87"/>
-      <c r="BC61" s="87"/>
-      <c r="BD61" s="87"/>
-      <c r="BE61" s="87"/>
-      <c r="BF61" s="87"/>
-      <c r="BG61" s="87"/>
-      <c r="BH61" s="87"/>
-      <c r="BI61" s="87"/>
-      <c r="BJ61" s="87"/>
-      <c r="BK61" s="87"/>
-      <c r="BL61" s="87"/>
-      <c r="BM61" s="87"/>
-      <c r="BN61" s="87"/>
-      <c r="BO61" s="148"/>
-      <c r="BP61" s="148"/>
-      <c r="BQ61" s="148"/>
-      <c r="BR61" s="148"/>
-      <c r="BS61" s="148"/>
-    </row>
-    <row r="62" spans="1:71" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="BO60" s="149"/>
+      <c r="BP60" s="149"/>
+      <c r="BQ60" s="149"/>
+      <c r="BR60" s="149"/>
+      <c r="BS60" s="149"/>
+    </row>
+    <row r="61" spans="1:71" s="51" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A61" s="49" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>7</v>
+      </c>
+      <c r="B61" s="50" t="s">
+        <v>172</v>
+      </c>
+      <c r="D61" s="52"/>
+      <c r="E61" s="84"/>
+      <c r="F61" s="84" t="str">
+        <f t="shared" ref="F61" si="38">IF(ISBLANK(E61)," - ",IF(G61=0,E61,E61+G61-1))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G61" s="53"/>
+      <c r="H61" s="54"/>
+      <c r="I61" s="55" t="str">
+        <f t="shared" ref="I61:I67" si="39">IF(OR(F61=0,E61=0)," - ",NETWORKDAYS(E61,F61))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J61" s="80"/>
+      <c r="K61" s="89"/>
+      <c r="L61" s="89"/>
+      <c r="M61" s="89"/>
+      <c r="N61" s="89"/>
+      <c r="O61" s="89"/>
+      <c r="P61" s="89"/>
+      <c r="Q61" s="89"/>
+      <c r="R61" s="89"/>
+      <c r="S61" s="89"/>
+      <c r="T61" s="89"/>
+      <c r="U61" s="89"/>
+      <c r="V61" s="89"/>
+      <c r="W61" s="89"/>
+      <c r="X61" s="89"/>
+      <c r="Y61" s="89"/>
+      <c r="Z61" s="89"/>
+      <c r="AA61" s="89"/>
+      <c r="AB61" s="89"/>
+      <c r="AC61" s="89"/>
+      <c r="AD61" s="89"/>
+      <c r="AE61" s="89"/>
+      <c r="AF61" s="89"/>
+      <c r="AG61" s="89"/>
+      <c r="AH61" s="89"/>
+      <c r="AI61" s="89"/>
+      <c r="AJ61" s="89"/>
+      <c r="AK61" s="89"/>
+      <c r="AL61" s="89"/>
+      <c r="AM61" s="89"/>
+      <c r="AN61" s="89"/>
+      <c r="AO61" s="89"/>
+      <c r="AP61" s="89"/>
+      <c r="AQ61" s="89"/>
+      <c r="AR61" s="89"/>
+      <c r="AS61" s="89"/>
+      <c r="AT61" s="89"/>
+      <c r="AU61" s="89"/>
+      <c r="AV61" s="89"/>
+      <c r="AW61" s="89"/>
+      <c r="AX61" s="89"/>
+      <c r="AY61" s="89"/>
+      <c r="AZ61" s="89"/>
+      <c r="BA61" s="89"/>
+      <c r="BB61" s="89"/>
+      <c r="BC61" s="89"/>
+      <c r="BD61" s="89"/>
+      <c r="BE61" s="89"/>
+      <c r="BF61" s="89"/>
+      <c r="BG61" s="89"/>
+      <c r="BH61" s="89"/>
+      <c r="BI61" s="89"/>
+      <c r="BJ61" s="89"/>
+      <c r="BK61" s="89"/>
+      <c r="BL61" s="89"/>
+      <c r="BM61" s="89"/>
+      <c r="BN61" s="89"/>
+    </row>
+    <row r="62" spans="1:71" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A62" s="56">
-        <v>7.7</v>
+        <v>7.1</v>
       </c>
       <c r="B62" s="106" t="s">
-        <v>155</v>
+        <v>173</v>
       </c>
       <c r="C62" s="57" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D62" s="107"/>
       <c r="E62" s="82">
-        <v>43920</v>
+        <v>43927</v>
       </c>
       <c r="F62" s="83">
-        <v>43924</v>
+        <v>43931</v>
       </c>
       <c r="G62" s="58">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H62" s="59">
         <v>0</v>
       </c>
       <c r="I62" s="60">
+        <f t="shared" si="39"/>
         <v>5</v>
       </c>
       <c r="J62" s="79"/>
@@ -9589,32 +9586,37 @@
       <c r="BL62" s="87"/>
       <c r="BM62" s="87"/>
       <c r="BN62" s="87"/>
+      <c r="BO62" s="148"/>
+      <c r="BP62" s="148"/>
+      <c r="BQ62" s="148"/>
+      <c r="BR62" s="148"/>
+      <c r="BS62" s="148"/>
     </row>
     <row r="63" spans="1:71" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A63" s="56">
-        <v>7.8</v>
+        <v>7.2</v>
       </c>
       <c r="B63" s="106" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="C63" s="57" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D63" s="107"/>
       <c r="E63" s="82">
-        <v>43920</v>
+        <v>43927</v>
       </c>
       <c r="F63" s="83">
-        <v>43924</v>
+        <v>43931</v>
       </c>
       <c r="G63" s="58">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H63" s="59">
         <v>0</v>
       </c>
       <c r="I63" s="60">
-        <f t="shared" ref="I63:I67" si="40">IF(OR(F63=0,E63=0)," - ",NETWORKDAYS(E63,F63))</f>
+        <f t="shared" si="39"/>
         <v>5</v>
       </c>
       <c r="J63" s="79"/>
@@ -9674,110 +9676,127 @@
       <c r="BL63" s="87"/>
       <c r="BM63" s="87"/>
       <c r="BN63" s="87"/>
-    </row>
-    <row r="64" spans="1:71" s="51" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A64" s="49" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>8</v>
-      </c>
-      <c r="B64" s="50" t="s">
-        <v>179</v>
-      </c>
-      <c r="D64" s="52"/>
-      <c r="E64" s="84"/>
-      <c r="F64" s="84" t="str">
-        <f t="shared" ref="F64" si="41">IF(ISBLANK(E64)," - ",IF(G64=0,E64,E64+G64-1))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G64" s="53"/>
-      <c r="H64" s="54"/>
-      <c r="I64" s="55" t="str">
-        <f t="shared" si="40"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J64" s="80"/>
-      <c r="K64" s="89"/>
-      <c r="L64" s="89"/>
-      <c r="M64" s="89"/>
-      <c r="N64" s="89"/>
-      <c r="O64" s="89"/>
-      <c r="P64" s="89"/>
-      <c r="Q64" s="89"/>
-      <c r="R64" s="89"/>
-      <c r="S64" s="89"/>
-      <c r="T64" s="89"/>
-      <c r="U64" s="89"/>
-      <c r="V64" s="89"/>
-      <c r="W64" s="89"/>
-      <c r="X64" s="89"/>
-      <c r="Y64" s="89"/>
-      <c r="Z64" s="89"/>
-      <c r="AA64" s="89"/>
-      <c r="AB64" s="89"/>
-      <c r="AC64" s="89"/>
-      <c r="AD64" s="89"/>
-      <c r="AE64" s="89"/>
-      <c r="AF64" s="89"/>
-      <c r="AG64" s="89"/>
-      <c r="AH64" s="89"/>
-      <c r="AI64" s="89"/>
-      <c r="AJ64" s="89"/>
-      <c r="AK64" s="89"/>
-      <c r="AL64" s="89"/>
-      <c r="AM64" s="89"/>
-      <c r="AN64" s="89"/>
-      <c r="AO64" s="89"/>
-      <c r="AP64" s="89"/>
-      <c r="AQ64" s="89"/>
-      <c r="AR64" s="89"/>
-      <c r="AS64" s="89"/>
-      <c r="AT64" s="89"/>
-      <c r="AU64" s="89"/>
-      <c r="AV64" s="89"/>
-      <c r="AW64" s="89"/>
-      <c r="AX64" s="89"/>
-      <c r="AY64" s="89"/>
-      <c r="AZ64" s="89"/>
-      <c r="BA64" s="89"/>
-      <c r="BB64" s="89"/>
-      <c r="BC64" s="89"/>
-      <c r="BD64" s="89"/>
-      <c r="BE64" s="89"/>
-      <c r="BF64" s="89"/>
-      <c r="BG64" s="89"/>
-      <c r="BH64" s="89"/>
-      <c r="BI64" s="89"/>
-      <c r="BJ64" s="89"/>
-      <c r="BK64" s="89"/>
-      <c r="BL64" s="89"/>
-      <c r="BM64" s="89"/>
-      <c r="BN64" s="89"/>
-    </row>
-    <row r="65" spans="1:83" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="BO63" s="148"/>
+      <c r="BP63" s="148"/>
+      <c r="BQ63" s="148"/>
+      <c r="BR63" s="148"/>
+      <c r="BS63" s="148"/>
+    </row>
+    <row r="64" spans="1:71" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A64" s="56">
+        <v>7.3</v>
+      </c>
+      <c r="B64" s="106" t="s">
+        <v>175</v>
+      </c>
+      <c r="C64" s="57" t="s">
+        <v>138</v>
+      </c>
+      <c r="D64" s="107"/>
+      <c r="E64" s="82">
+        <v>43927</v>
+      </c>
+      <c r="F64" s="83">
+        <v>43931</v>
+      </c>
+      <c r="G64" s="58">
+        <v>2</v>
+      </c>
+      <c r="H64" s="59">
+        <v>0</v>
+      </c>
+      <c r="I64" s="60">
+        <f t="shared" si="39"/>
+        <v>5</v>
+      </c>
+      <c r="J64" s="79"/>
+      <c r="K64" s="87"/>
+      <c r="L64" s="87"/>
+      <c r="M64" s="87"/>
+      <c r="N64" s="87"/>
+      <c r="O64" s="87"/>
+      <c r="P64" s="87"/>
+      <c r="Q64" s="87"/>
+      <c r="R64" s="87"/>
+      <c r="S64" s="87"/>
+      <c r="T64" s="87"/>
+      <c r="U64" s="87"/>
+      <c r="V64" s="87"/>
+      <c r="W64" s="87"/>
+      <c r="X64" s="87"/>
+      <c r="Y64" s="87"/>
+      <c r="Z64" s="87"/>
+      <c r="AA64" s="87"/>
+      <c r="AB64" s="87"/>
+      <c r="AC64" s="87"/>
+      <c r="AD64" s="87"/>
+      <c r="AE64" s="87"/>
+      <c r="AF64" s="87"/>
+      <c r="AG64" s="87"/>
+      <c r="AH64" s="87"/>
+      <c r="AI64" s="87"/>
+      <c r="AJ64" s="87"/>
+      <c r="AK64" s="87"/>
+      <c r="AL64" s="87"/>
+      <c r="AM64" s="87"/>
+      <c r="AN64" s="87"/>
+      <c r="AO64" s="87"/>
+      <c r="AP64" s="87"/>
+      <c r="AQ64" s="87"/>
+      <c r="AR64" s="87"/>
+      <c r="AS64" s="87"/>
+      <c r="AT64" s="87"/>
+      <c r="AU64" s="87"/>
+      <c r="AV64" s="87"/>
+      <c r="AW64" s="87"/>
+      <c r="AX64" s="87"/>
+      <c r="AY64" s="87"/>
+      <c r="AZ64" s="87"/>
+      <c r="BA64" s="87"/>
+      <c r="BB64" s="87"/>
+      <c r="BC64" s="87"/>
+      <c r="BD64" s="87"/>
+      <c r="BE64" s="87"/>
+      <c r="BF64" s="87"/>
+      <c r="BG64" s="87"/>
+      <c r="BH64" s="87"/>
+      <c r="BI64" s="87"/>
+      <c r="BJ64" s="87"/>
+      <c r="BK64" s="87"/>
+      <c r="BL64" s="87"/>
+      <c r="BM64" s="87"/>
+      <c r="BN64" s="87"/>
+      <c r="BO64" s="148"/>
+      <c r="BP64" s="148"/>
+      <c r="BQ64" s="148"/>
+      <c r="BR64" s="148"/>
+      <c r="BS64" s="148"/>
+    </row>
+    <row r="65" spans="1:83" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A65" s="56">
-        <v>6.1</v>
+        <v>7.4</v>
       </c>
       <c r="B65" s="106" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C65" s="57" t="s">
-        <v>163</v>
+        <v>138</v>
       </c>
       <c r="D65" s="107"/>
       <c r="E65" s="82">
-        <v>43934</v>
+        <v>43927</v>
       </c>
       <c r="F65" s="83">
-        <v>43940</v>
+        <v>43931</v>
       </c>
       <c r="G65" s="58">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H65" s="59">
         <v>0</v>
       </c>
       <c r="I65" s="60">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>5</v>
       </c>
       <c r="J65" s="79"/>
@@ -9837,38 +9856,37 @@
       <c r="BL65" s="87"/>
       <c r="BM65" s="87"/>
       <c r="BN65" s="87"/>
-      <c r="BV65" s="148"/>
-      <c r="BW65" s="148"/>
-      <c r="BX65" s="148"/>
-      <c r="BY65" s="148"/>
-      <c r="BZ65" s="148"/>
-      <c r="CE65" s="149"/>
-    </row>
-    <row r="66" spans="1:83" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="BO65" s="148"/>
+      <c r="BP65" s="148"/>
+      <c r="BQ65" s="148"/>
+      <c r="BR65" s="148"/>
+      <c r="BS65" s="148"/>
+    </row>
+    <row r="66" spans="1:83" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A66" s="56">
-        <v>6.2</v>
+        <v>7.5</v>
       </c>
       <c r="B66" s="106" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C66" s="57" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="D66" s="107"/>
       <c r="E66" s="82">
-        <v>43934</v>
+        <v>43927</v>
       </c>
       <c r="F66" s="83">
-        <v>43940</v>
+        <v>43931</v>
       </c>
       <c r="G66" s="58">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H66" s="59">
         <v>0</v>
       </c>
       <c r="I66" s="60">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>5</v>
       </c>
       <c r="J66" s="79"/>
@@ -9928,38 +9946,37 @@
       <c r="BL66" s="87"/>
       <c r="BM66" s="87"/>
       <c r="BN66" s="87"/>
-      <c r="BV66" s="148"/>
-      <c r="BW66" s="148"/>
-      <c r="BX66" s="148"/>
-      <c r="BY66" s="148"/>
-      <c r="BZ66" s="148"/>
-      <c r="CE66" s="149"/>
-    </row>
-    <row r="67" spans="1:83" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="BO66" s="148"/>
+      <c r="BP66" s="148"/>
+      <c r="BQ66" s="148"/>
+      <c r="BR66" s="148"/>
+      <c r="BS66" s="148"/>
+    </row>
+    <row r="67" spans="1:83" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A67" s="56">
-        <v>6.3</v>
+        <v>7.6</v>
       </c>
       <c r="B67" s="106" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C67" s="57" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="D67" s="107"/>
       <c r="E67" s="82">
-        <v>43934</v>
+        <v>43927</v>
       </c>
       <c r="F67" s="83">
-        <v>43940</v>
+        <v>43931</v>
       </c>
       <c r="G67" s="58">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H67" s="59">
         <v>0</v>
       </c>
       <c r="I67" s="60">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>5</v>
       </c>
       <c r="J67" s="79"/>
@@ -10019,27 +10036,39 @@
       <c r="BL67" s="87"/>
       <c r="BM67" s="87"/>
       <c r="BN67" s="87"/>
-      <c r="BV67" s="148"/>
-      <c r="BW67" s="148"/>
-      <c r="BX67" s="148"/>
-      <c r="BY67" s="148"/>
-      <c r="BZ67" s="148"/>
-      <c r="CE67" s="149"/>
-    </row>
-    <row r="68" spans="1:83" s="66" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A68" s="56"/>
-      <c r="B68" s="61"/>
-      <c r="C68" s="61"/>
-      <c r="D68" s="62"/>
-      <c r="E68" s="85"/>
-      <c r="F68" s="85"/>
-      <c r="G68" s="63"/>
-      <c r="H68" s="64"/>
-      <c r="I68" s="65" t="str">
-        <f t="shared" si="31"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J68" s="81"/>
+      <c r="BO67" s="148"/>
+      <c r="BP67" s="148"/>
+      <c r="BQ67" s="148"/>
+      <c r="BR67" s="148"/>
+      <c r="BS67" s="148"/>
+    </row>
+    <row r="68" spans="1:83" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A68" s="56">
+        <v>7.7</v>
+      </c>
+      <c r="B68" s="106" t="s">
+        <v>155</v>
+      </c>
+      <c r="C68" s="57" t="s">
+        <v>143</v>
+      </c>
+      <c r="D68" s="107"/>
+      <c r="E68" s="82">
+        <v>43920</v>
+      </c>
+      <c r="F68" s="83">
+        <v>43924</v>
+      </c>
+      <c r="G68" s="58">
+        <v>1</v>
+      </c>
+      <c r="H68" s="59">
+        <v>0</v>
+      </c>
+      <c r="I68" s="60">
+        <v>5</v>
+      </c>
+      <c r="J68" s="79"/>
       <c r="K68" s="87"/>
       <c r="L68" s="87"/>
       <c r="M68" s="87"/>
@@ -10097,20 +10126,34 @@
       <c r="BM68" s="87"/>
       <c r="BN68" s="87"/>
     </row>
-    <row r="69" spans="1:83" s="66" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A69" s="56"/>
-      <c r="B69" s="61"/>
-      <c r="C69" s="61"/>
-      <c r="D69" s="62"/>
-      <c r="E69" s="85"/>
-      <c r="F69" s="85"/>
-      <c r="G69" s="63"/>
-      <c r="H69" s="64"/>
-      <c r="I69" s="65" t="str">
-        <f t="shared" si="31"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J69" s="81"/>
+    <row r="69" spans="1:83" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A69" s="56">
+        <v>7.8</v>
+      </c>
+      <c r="B69" s="106" t="s">
+        <v>154</v>
+      </c>
+      <c r="C69" s="57" t="s">
+        <v>138</v>
+      </c>
+      <c r="D69" s="107"/>
+      <c r="E69" s="82">
+        <v>43920</v>
+      </c>
+      <c r="F69" s="83">
+        <v>43924</v>
+      </c>
+      <c r="G69" s="58">
+        <v>1</v>
+      </c>
+      <c r="H69" s="59">
+        <v>0</v>
+      </c>
+      <c r="I69" s="60">
+        <f t="shared" ref="I69:I73" si="40">IF(OR(F69=0,E69=0)," - ",NETWORKDAYS(E69,F69))</f>
+        <v>5</v>
+      </c>
+      <c r="J69" s="79"/>
       <c r="K69" s="87"/>
       <c r="L69" s="87"/>
       <c r="M69" s="87"/>
@@ -10168,6 +10211,499 @@
       <c r="BM69" s="87"/>
       <c r="BN69" s="87"/>
     </row>
+    <row r="70" spans="1:83" s="51" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A70" s="49" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>8</v>
+      </c>
+      <c r="B70" s="50" t="s">
+        <v>179</v>
+      </c>
+      <c r="D70" s="52"/>
+      <c r="E70" s="84"/>
+      <c r="F70" s="84" t="str">
+        <f t="shared" ref="F70" si="41">IF(ISBLANK(E70)," - ",IF(G70=0,E70,E70+G70-1))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G70" s="53"/>
+      <c r="H70" s="54"/>
+      <c r="I70" s="55" t="str">
+        <f t="shared" si="40"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J70" s="80"/>
+      <c r="K70" s="89"/>
+      <c r="L70" s="89"/>
+      <c r="M70" s="89"/>
+      <c r="N70" s="89"/>
+      <c r="O70" s="89"/>
+      <c r="P70" s="89"/>
+      <c r="Q70" s="89"/>
+      <c r="R70" s="89"/>
+      <c r="S70" s="89"/>
+      <c r="T70" s="89"/>
+      <c r="U70" s="89"/>
+      <c r="V70" s="89"/>
+      <c r="W70" s="89"/>
+      <c r="X70" s="89"/>
+      <c r="Y70" s="89"/>
+      <c r="Z70" s="89"/>
+      <c r="AA70" s="89"/>
+      <c r="AB70" s="89"/>
+      <c r="AC70" s="89"/>
+      <c r="AD70" s="89"/>
+      <c r="AE70" s="89"/>
+      <c r="AF70" s="89"/>
+      <c r="AG70" s="89"/>
+      <c r="AH70" s="89"/>
+      <c r="AI70" s="89"/>
+      <c r="AJ70" s="89"/>
+      <c r="AK70" s="89"/>
+      <c r="AL70" s="89"/>
+      <c r="AM70" s="89"/>
+      <c r="AN70" s="89"/>
+      <c r="AO70" s="89"/>
+      <c r="AP70" s="89"/>
+      <c r="AQ70" s="89"/>
+      <c r="AR70" s="89"/>
+      <c r="AS70" s="89"/>
+      <c r="AT70" s="89"/>
+      <c r="AU70" s="89"/>
+      <c r="AV70" s="89"/>
+      <c r="AW70" s="89"/>
+      <c r="AX70" s="89"/>
+      <c r="AY70" s="89"/>
+      <c r="AZ70" s="89"/>
+      <c r="BA70" s="89"/>
+      <c r="BB70" s="89"/>
+      <c r="BC70" s="89"/>
+      <c r="BD70" s="89"/>
+      <c r="BE70" s="89"/>
+      <c r="BF70" s="89"/>
+      <c r="BG70" s="89"/>
+      <c r="BH70" s="89"/>
+      <c r="BI70" s="89"/>
+      <c r="BJ70" s="89"/>
+      <c r="BK70" s="89"/>
+      <c r="BL70" s="89"/>
+      <c r="BM70" s="89"/>
+      <c r="BN70" s="89"/>
+    </row>
+    <row r="71" spans="1:83" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A71" s="56">
+        <v>6.1</v>
+      </c>
+      <c r="B71" s="106" t="s">
+        <v>180</v>
+      </c>
+      <c r="C71" s="57" t="s">
+        <v>163</v>
+      </c>
+      <c r="D71" s="107"/>
+      <c r="E71" s="82">
+        <v>43934</v>
+      </c>
+      <c r="F71" s="83">
+        <v>43940</v>
+      </c>
+      <c r="G71" s="58">
+        <v>5</v>
+      </c>
+      <c r="H71" s="59">
+        <v>0</v>
+      </c>
+      <c r="I71" s="60">
+        <f t="shared" si="40"/>
+        <v>5</v>
+      </c>
+      <c r="J71" s="79"/>
+      <c r="K71" s="87"/>
+      <c r="L71" s="87"/>
+      <c r="M71" s="87"/>
+      <c r="N71" s="87"/>
+      <c r="O71" s="87"/>
+      <c r="P71" s="87"/>
+      <c r="Q71" s="87"/>
+      <c r="R71" s="87"/>
+      <c r="S71" s="87"/>
+      <c r="T71" s="87"/>
+      <c r="U71" s="87"/>
+      <c r="V71" s="87"/>
+      <c r="W71" s="87"/>
+      <c r="X71" s="87"/>
+      <c r="Y71" s="87"/>
+      <c r="Z71" s="87"/>
+      <c r="AA71" s="87"/>
+      <c r="AB71" s="87"/>
+      <c r="AC71" s="87"/>
+      <c r="AD71" s="87"/>
+      <c r="AE71" s="87"/>
+      <c r="AF71" s="87"/>
+      <c r="AG71" s="87"/>
+      <c r="AH71" s="87"/>
+      <c r="AI71" s="87"/>
+      <c r="AJ71" s="87"/>
+      <c r="AK71" s="87"/>
+      <c r="AL71" s="87"/>
+      <c r="AM71" s="87"/>
+      <c r="AN71" s="87"/>
+      <c r="AO71" s="87"/>
+      <c r="AP71" s="87"/>
+      <c r="AQ71" s="87"/>
+      <c r="AR71" s="87"/>
+      <c r="AS71" s="87"/>
+      <c r="AT71" s="87"/>
+      <c r="AU71" s="87"/>
+      <c r="AV71" s="87"/>
+      <c r="AW71" s="87"/>
+      <c r="AX71" s="87"/>
+      <c r="AY71" s="87"/>
+      <c r="AZ71" s="87"/>
+      <c r="BA71" s="87"/>
+      <c r="BB71" s="87"/>
+      <c r="BC71" s="87"/>
+      <c r="BD71" s="87"/>
+      <c r="BE71" s="87"/>
+      <c r="BF71" s="87"/>
+      <c r="BG71" s="87"/>
+      <c r="BH71" s="87"/>
+      <c r="BI71" s="87"/>
+      <c r="BJ71" s="87"/>
+      <c r="BK71" s="87"/>
+      <c r="BL71" s="87"/>
+      <c r="BM71" s="87"/>
+      <c r="BN71" s="87"/>
+      <c r="BV71" s="148"/>
+      <c r="BW71" s="148"/>
+      <c r="BX71" s="148"/>
+      <c r="BY71" s="148"/>
+      <c r="BZ71" s="148"/>
+      <c r="CE71" s="149"/>
+    </row>
+    <row r="72" spans="1:83" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A72" s="56">
+        <v>6.2</v>
+      </c>
+      <c r="B72" s="106" t="s">
+        <v>181</v>
+      </c>
+      <c r="C72" s="57" t="s">
+        <v>163</v>
+      </c>
+      <c r="D72" s="107"/>
+      <c r="E72" s="82">
+        <v>43934</v>
+      </c>
+      <c r="F72" s="83">
+        <v>43940</v>
+      </c>
+      <c r="G72" s="58">
+        <v>5</v>
+      </c>
+      <c r="H72" s="59">
+        <v>0</v>
+      </c>
+      <c r="I72" s="60">
+        <f t="shared" si="40"/>
+        <v>5</v>
+      </c>
+      <c r="J72" s="79"/>
+      <c r="K72" s="87"/>
+      <c r="L72" s="87"/>
+      <c r="M72" s="87"/>
+      <c r="N72" s="87"/>
+      <c r="O72" s="87"/>
+      <c r="P72" s="87"/>
+      <c r="Q72" s="87"/>
+      <c r="R72" s="87"/>
+      <c r="S72" s="87"/>
+      <c r="T72" s="87"/>
+      <c r="U72" s="87"/>
+      <c r="V72" s="87"/>
+      <c r="W72" s="87"/>
+      <c r="X72" s="87"/>
+      <c r="Y72" s="87"/>
+      <c r="Z72" s="87"/>
+      <c r="AA72" s="87"/>
+      <c r="AB72" s="87"/>
+      <c r="AC72" s="87"/>
+      <c r="AD72" s="87"/>
+      <c r="AE72" s="87"/>
+      <c r="AF72" s="87"/>
+      <c r="AG72" s="87"/>
+      <c r="AH72" s="87"/>
+      <c r="AI72" s="87"/>
+      <c r="AJ72" s="87"/>
+      <c r="AK72" s="87"/>
+      <c r="AL72" s="87"/>
+      <c r="AM72" s="87"/>
+      <c r="AN72" s="87"/>
+      <c r="AO72" s="87"/>
+      <c r="AP72" s="87"/>
+      <c r="AQ72" s="87"/>
+      <c r="AR72" s="87"/>
+      <c r="AS72" s="87"/>
+      <c r="AT72" s="87"/>
+      <c r="AU72" s="87"/>
+      <c r="AV72" s="87"/>
+      <c r="AW72" s="87"/>
+      <c r="AX72" s="87"/>
+      <c r="AY72" s="87"/>
+      <c r="AZ72" s="87"/>
+      <c r="BA72" s="87"/>
+      <c r="BB72" s="87"/>
+      <c r="BC72" s="87"/>
+      <c r="BD72" s="87"/>
+      <c r="BE72" s="87"/>
+      <c r="BF72" s="87"/>
+      <c r="BG72" s="87"/>
+      <c r="BH72" s="87"/>
+      <c r="BI72" s="87"/>
+      <c r="BJ72" s="87"/>
+      <c r="BK72" s="87"/>
+      <c r="BL72" s="87"/>
+      <c r="BM72" s="87"/>
+      <c r="BN72" s="87"/>
+      <c r="BV72" s="148"/>
+      <c r="BW72" s="148"/>
+      <c r="BX72" s="148"/>
+      <c r="BY72" s="148"/>
+      <c r="BZ72" s="148"/>
+      <c r="CE72" s="149"/>
+    </row>
+    <row r="73" spans="1:83" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A73" s="56">
+        <v>6.3</v>
+      </c>
+      <c r="B73" s="106" t="s">
+        <v>182</v>
+      </c>
+      <c r="C73" s="57" t="s">
+        <v>163</v>
+      </c>
+      <c r="D73" s="107"/>
+      <c r="E73" s="82">
+        <v>43934</v>
+      </c>
+      <c r="F73" s="83">
+        <v>43940</v>
+      </c>
+      <c r="G73" s="58">
+        <v>5</v>
+      </c>
+      <c r="H73" s="59">
+        <v>0</v>
+      </c>
+      <c r="I73" s="60">
+        <f t="shared" si="40"/>
+        <v>5</v>
+      </c>
+      <c r="J73" s="79"/>
+      <c r="K73" s="87"/>
+      <c r="L73" s="87"/>
+      <c r="M73" s="87"/>
+      <c r="N73" s="87"/>
+      <c r="O73" s="87"/>
+      <c r="P73" s="87"/>
+      <c r="Q73" s="87"/>
+      <c r="R73" s="87"/>
+      <c r="S73" s="87"/>
+      <c r="T73" s="87"/>
+      <c r="U73" s="87"/>
+      <c r="V73" s="87"/>
+      <c r="W73" s="87"/>
+      <c r="X73" s="87"/>
+      <c r="Y73" s="87"/>
+      <c r="Z73" s="87"/>
+      <c r="AA73" s="87"/>
+      <c r="AB73" s="87"/>
+      <c r="AC73" s="87"/>
+      <c r="AD73" s="87"/>
+      <c r="AE73" s="87"/>
+      <c r="AF73" s="87"/>
+      <c r="AG73" s="87"/>
+      <c r="AH73" s="87"/>
+      <c r="AI73" s="87"/>
+      <c r="AJ73" s="87"/>
+      <c r="AK73" s="87"/>
+      <c r="AL73" s="87"/>
+      <c r="AM73" s="87"/>
+      <c r="AN73" s="87"/>
+      <c r="AO73" s="87"/>
+      <c r="AP73" s="87"/>
+      <c r="AQ73" s="87"/>
+      <c r="AR73" s="87"/>
+      <c r="AS73" s="87"/>
+      <c r="AT73" s="87"/>
+      <c r="AU73" s="87"/>
+      <c r="AV73" s="87"/>
+      <c r="AW73" s="87"/>
+      <c r="AX73" s="87"/>
+      <c r="AY73" s="87"/>
+      <c r="AZ73" s="87"/>
+      <c r="BA73" s="87"/>
+      <c r="BB73" s="87"/>
+      <c r="BC73" s="87"/>
+      <c r="BD73" s="87"/>
+      <c r="BE73" s="87"/>
+      <c r="BF73" s="87"/>
+      <c r="BG73" s="87"/>
+      <c r="BH73" s="87"/>
+      <c r="BI73" s="87"/>
+      <c r="BJ73" s="87"/>
+      <c r="BK73" s="87"/>
+      <c r="BL73" s="87"/>
+      <c r="BM73" s="87"/>
+      <c r="BN73" s="87"/>
+      <c r="BV73" s="148"/>
+      <c r="BW73" s="148"/>
+      <c r="BX73" s="148"/>
+      <c r="BY73" s="148"/>
+      <c r="BZ73" s="148"/>
+      <c r="CE73" s="149"/>
+    </row>
+    <row r="74" spans="1:83" s="66" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A74" s="56"/>
+      <c r="B74" s="61"/>
+      <c r="C74" s="61"/>
+      <c r="D74" s="62"/>
+      <c r="E74" s="85"/>
+      <c r="F74" s="85"/>
+      <c r="G74" s="63"/>
+      <c r="H74" s="64"/>
+      <c r="I74" s="65" t="str">
+        <f t="shared" si="31"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J74" s="81"/>
+      <c r="K74" s="87"/>
+      <c r="L74" s="87"/>
+      <c r="M74" s="87"/>
+      <c r="N74" s="87"/>
+      <c r="O74" s="87"/>
+      <c r="P74" s="87"/>
+      <c r="Q74" s="87"/>
+      <c r="R74" s="87"/>
+      <c r="S74" s="87"/>
+      <c r="T74" s="87"/>
+      <c r="U74" s="87"/>
+      <c r="V74" s="87"/>
+      <c r="W74" s="87"/>
+      <c r="X74" s="87"/>
+      <c r="Y74" s="87"/>
+      <c r="Z74" s="87"/>
+      <c r="AA74" s="87"/>
+      <c r="AB74" s="87"/>
+      <c r="AC74" s="87"/>
+      <c r="AD74" s="87"/>
+      <c r="AE74" s="87"/>
+      <c r="AF74" s="87"/>
+      <c r="AG74" s="87"/>
+      <c r="AH74" s="87"/>
+      <c r="AI74" s="87"/>
+      <c r="AJ74" s="87"/>
+      <c r="AK74" s="87"/>
+      <c r="AL74" s="87"/>
+      <c r="AM74" s="87"/>
+      <c r="AN74" s="87"/>
+      <c r="AO74" s="87"/>
+      <c r="AP74" s="87"/>
+      <c r="AQ74" s="87"/>
+      <c r="AR74" s="87"/>
+      <c r="AS74" s="87"/>
+      <c r="AT74" s="87"/>
+      <c r="AU74" s="87"/>
+      <c r="AV74" s="87"/>
+      <c r="AW74" s="87"/>
+      <c r="AX74" s="87"/>
+      <c r="AY74" s="87"/>
+      <c r="AZ74" s="87"/>
+      <c r="BA74" s="87"/>
+      <c r="BB74" s="87"/>
+      <c r="BC74" s="87"/>
+      <c r="BD74" s="87"/>
+      <c r="BE74" s="87"/>
+      <c r="BF74" s="87"/>
+      <c r="BG74" s="87"/>
+      <c r="BH74" s="87"/>
+      <c r="BI74" s="87"/>
+      <c r="BJ74" s="87"/>
+      <c r="BK74" s="87"/>
+      <c r="BL74" s="87"/>
+      <c r="BM74" s="87"/>
+      <c r="BN74" s="87"/>
+    </row>
+    <row r="75" spans="1:83" s="66" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A75" s="56"/>
+      <c r="B75" s="61"/>
+      <c r="C75" s="61"/>
+      <c r="D75" s="62"/>
+      <c r="E75" s="85"/>
+      <c r="F75" s="85"/>
+      <c r="G75" s="63"/>
+      <c r="H75" s="64"/>
+      <c r="I75" s="65" t="str">
+        <f t="shared" si="31"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J75" s="81"/>
+      <c r="K75" s="87"/>
+      <c r="L75" s="87"/>
+      <c r="M75" s="87"/>
+      <c r="N75" s="87"/>
+      <c r="O75" s="87"/>
+      <c r="P75" s="87"/>
+      <c r="Q75" s="87"/>
+      <c r="R75" s="87"/>
+      <c r="S75" s="87"/>
+      <c r="T75" s="87"/>
+      <c r="U75" s="87"/>
+      <c r="V75" s="87"/>
+      <c r="W75" s="87"/>
+      <c r="X75" s="87"/>
+      <c r="Y75" s="87"/>
+      <c r="Z75" s="87"/>
+      <c r="AA75" s="87"/>
+      <c r="AB75" s="87"/>
+      <c r="AC75" s="87"/>
+      <c r="AD75" s="87"/>
+      <c r="AE75" s="87"/>
+      <c r="AF75" s="87"/>
+      <c r="AG75" s="87"/>
+      <c r="AH75" s="87"/>
+      <c r="AI75" s="87"/>
+      <c r="AJ75" s="87"/>
+      <c r="AK75" s="87"/>
+      <c r="AL75" s="87"/>
+      <c r="AM75" s="87"/>
+      <c r="AN75" s="87"/>
+      <c r="AO75" s="87"/>
+      <c r="AP75" s="87"/>
+      <c r="AQ75" s="87"/>
+      <c r="AR75" s="87"/>
+      <c r="AS75" s="87"/>
+      <c r="AT75" s="87"/>
+      <c r="AU75" s="87"/>
+      <c r="AV75" s="87"/>
+      <c r="AW75" s="87"/>
+      <c r="AX75" s="87"/>
+      <c r="AY75" s="87"/>
+      <c r="AZ75" s="87"/>
+      <c r="BA75" s="87"/>
+      <c r="BB75" s="87"/>
+      <c r="BC75" s="87"/>
+      <c r="BD75" s="87"/>
+      <c r="BE75" s="87"/>
+      <c r="BF75" s="87"/>
+      <c r="BG75" s="87"/>
+      <c r="BH75" s="87"/>
+      <c r="BI75" s="87"/>
+      <c r="BJ75" s="87"/>
+      <c r="BK75" s="87"/>
+      <c r="BL75" s="87"/>
+      <c r="BM75" s="87"/>
+      <c r="BN75" s="87"/>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="25">
@@ -10198,7 +10734,7 @@
     <mergeCell ref="Y5:AE5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="H68:H69 H8:H54">
+  <conditionalFormatting sqref="H74:H75 H8:H60">
     <cfRule type="dataBar" priority="22">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -10217,7 +10753,7 @@
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K8:BN69">
+  <conditionalFormatting sqref="K8:BN75">
     <cfRule type="expression" dxfId="5" priority="68">
       <formula>AND($E8&lt;=K$6,ROUNDDOWN(($F8-$E8+1)*$H8,0)+$E8-1&gt;=K$6)</formula>
     </cfRule>
@@ -10225,12 +10761,12 @@
       <formula>AND(NOT(ISBLANK($E8)),$E8&lt;=K$6,$F8&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K68:BN69 BO6:CI7 K6:BN54">
+  <conditionalFormatting sqref="K74:BN75 BO6:CI7 K6:BN60">
     <cfRule type="expression" dxfId="3" priority="28">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H55:H62">
+  <conditionalFormatting sqref="H61:H68">
     <cfRule type="dataBar" priority="13">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -10244,12 +10780,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K55:BN62">
+  <conditionalFormatting sqref="K61:BN68">
     <cfRule type="expression" dxfId="2" priority="14">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H63">
+  <conditionalFormatting sqref="H69">
     <cfRule type="dataBar" priority="9">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -10263,12 +10799,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K63:BN63">
+  <conditionalFormatting sqref="K69:BN69">
     <cfRule type="expression" dxfId="1" priority="10">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H64:H67">
+  <conditionalFormatting sqref="H70:H73">
     <cfRule type="dataBar" priority="5">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -10282,7 +10818,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K64:BN67">
+  <conditionalFormatting sqref="K70:BN73">
     <cfRule type="expression" dxfId="0" priority="6">
       <formula>K$6=TODAY()</formula>
     </cfRule>
@@ -10297,8 +10833,8 @@
   <pageSetup scale="63" fitToHeight="0" orientation="landscape" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <ignoredErrors>
-    <ignoredError sqref="H9 A69:B69 E16 E27 E36 E68:H69 G16:H16 G27:H27 G36:H36 H33 G39:H39 H40 H37:H38 A68 H28:H29" unlockedFormula="1"/>
-    <ignoredError sqref="A36 A27 A16" formula="1"/>
+    <ignoredError sqref="H9 A75:B75 E16 E33 E42 E74:H75 G16:H16 G33:H33 G42:H42 H39 G45:H45 H43:H44 A74" unlockedFormula="1"/>
+    <ignoredError sqref="A42 A33 A16" formula="1"/>
   </ignoredErrors>
   <drawing r:id="rId3"/>
   <legacyDrawing r:id="rId4"/>
@@ -10346,7 +10882,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H68:H69 H8:H54</xm:sqref>
+          <xm:sqref>H74:H75 H8:H60</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{0F99DC93-F37E-44FD-BA80-440E3A4D599D}">
@@ -10361,7 +10897,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H55:H62</xm:sqref>
+          <xm:sqref>H61:H68</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{B9031F11-912A-4A5C-85BD-BFB059CEAD5B}">
@@ -10376,7 +10912,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H63</xm:sqref>
+          <xm:sqref>H69</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{437A52F8-D2E6-4093-9466-950C3C255C94}">
@@ -10391,7 +10927,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H64:H67</xm:sqref>
+          <xm:sqref>H70:H73</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>